<commit_message>
tiva properly receiving and storing data
</commit_message>
<xml_diff>
--- a/Command_Data Planner.xlsx
+++ b/Command_Data Planner.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Materia\2022 Spring\Courses\ECPE-155 Autonomous Robotics\Labs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emily\bishop_ecpe155_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3765E0-0EF6-4A0D-B32C-758BB285F71E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C2F2F6-692C-4BA6-B406-DC9EE6F5257E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{41C8675F-361B-4635-AFD0-4B5E8933C9D2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{41C8675F-361B-4635-AFD0-4B5E8933C9D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t xml:space="preserve">command </t>
   </si>
@@ -110,13 +110,55 @@
   </si>
   <si>
     <t>0x55</t>
+  </si>
+  <si>
+    <t>Hex</t>
+  </si>
+  <si>
+    <t>0x81</t>
+  </si>
+  <si>
+    <t>0x82</t>
+  </si>
+  <si>
+    <t>0x83</t>
+  </si>
+  <si>
+    <t>0x84</t>
+  </si>
+  <si>
+    <t>0x85</t>
+  </si>
+  <si>
+    <t>0x86</t>
+  </si>
+  <si>
+    <t>0x87</t>
+  </si>
+  <si>
+    <t>0x88</t>
+  </si>
+  <si>
+    <t>0x40</t>
+  </si>
+  <si>
+    <t>0x41</t>
+  </si>
+  <si>
+    <t>0x42</t>
+  </si>
+  <si>
+    <t>0x43</t>
+  </si>
+  <si>
+    <t>0x44</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +171,12 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -519,22 +567,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6836315B-2C81-4F83-8718-E67FA02C11DA}">
-  <dimension ref="A1:AA40"/>
+  <dimension ref="A1:AD40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:A40"/>
+      <selection activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="9.140625" style="1"/>
-    <col min="10" max="10" width="10.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="2"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="22.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="9.109375" style="1"/>
+    <col min="10" max="10" width="10.5546875" style="1" customWidth="1"/>
+    <col min="11" max="13" width="10.5546875" style="7" customWidth="1"/>
+    <col min="14" max="14" width="9.109375" style="2"/>
+    <col min="15" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -562,14 +611,17 @@
       <c r="J1" s="1">
         <v>0</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="L1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -582,16 +634,13 @@
       <c r="D2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="8"/>
-      <c r="M2" s="1" t="s">
+      <c r="O2" s="8"/>
+      <c r="P2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
       <c r="R2" s="8"/>
       <c r="S2" s="8"/>
       <c r="T2" s="8"/>
@@ -602,8 +651,11 @@
       <c r="Y2" s="8"/>
       <c r="Z2" s="8"/>
       <c r="AA2" s="8"/>
-    </row>
-    <row r="3" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
+      <c r="AD2" s="8"/>
+    </row>
+    <row r="3" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -619,9 +671,9 @@
       <c r="E3" s="6">
         <v>0</v>
       </c>
-      <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -649,9 +701,9 @@
       <c r="J4" s="4">
         <v>0</v>
       </c>
-      <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -680,8 +732,11 @@
       <c r="J5" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="L5" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -710,8 +765,11 @@
       <c r="J6" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="L6" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
@@ -740,8 +798,11 @@
       <c r="J7" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="L7" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -770,8 +831,11 @@
       <c r="J8" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="L8" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
@@ -800,8 +864,11 @@
       <c r="J9" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="L9" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -830,8 +897,11 @@
       <c r="J10" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="L10" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
@@ -860,8 +930,11 @@
       <c r="J11" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="L11" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
@@ -890,8 +963,11 @@
       <c r="J12" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="L12" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -911,7 +987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -931,7 +1007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -951,7 +1027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -971,7 +1047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -991,7 +1067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -1011,7 +1087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -1031,7 +1107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -1043,7 +1119,7 @@
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -1055,7 +1131,7 @@
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -1067,7 +1143,7 @@
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
     </row>
-    <row r="24" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>3</v>
       </c>
@@ -1083,9 +1159,9 @@
       <c r="E24" s="6">
         <v>0</v>
       </c>
-      <c r="K24" s="2"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N24" s="2"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>15</v>
       </c>
@@ -1113,8 +1189,11 @@
       <c r="J25" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>16</v>
       </c>
@@ -1142,8 +1221,11 @@
       <c r="J26" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>17</v>
       </c>
@@ -1171,8 +1253,11 @@
       <c r="J27" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>18</v>
       </c>
@@ -1200,8 +1285,11 @@
       <c r="J28" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L28" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>19</v>
       </c>
@@ -1229,8 +1317,11 @@
       <c r="J29" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L29" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="G30" s="4">
         <v>0</v>
@@ -1245,7 +1336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="G31" s="4">
         <v>0</v>
@@ -1260,7 +1351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="G32" s="4">
         <v>0</v>
@@ -1275,7 +1366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="G33" s="4">
         <v>1</v>
@@ -1290,7 +1381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="G34" s="4">
         <v>1</v>
@@ -1305,7 +1396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="G35" s="4">
         <v>1</v>
@@ -1320,7 +1411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="G36" s="4">
         <v>1</v>
@@ -1335,7 +1426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="G37" s="4">
         <v>1</v>
@@ -1350,7 +1441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="G38" s="4">
         <v>1</v>
@@ -1365,7 +1456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="G39" s="4">
         <v>1</v>
@@ -1380,7 +1471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="4"/>
       <c r="G40" s="4">
         <v>1</v>
@@ -1396,6 +1487,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
new packet protocol plans. Lab6 prepped for implementing motorforward and IR data transmission
</commit_message>
<xml_diff>
--- a/Command_Data Planner.xlsx
+++ b/Command_Data Planner.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emily\bishop_ecpe155_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C2F2F6-692C-4BA6-B406-DC9EE6F5257E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF4C5AF-CF1B-4CD7-9475-8260293422F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{41C8675F-361B-4635-AFD0-4B5E8933C9D2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Packet Protocol" sheetId="4" r:id="rId1"/>
+    <sheet name="OG protocol" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="78">
   <si>
     <t xml:space="preserve">command </t>
   </si>
@@ -152,6 +153,123 @@
   </si>
   <si>
     <t>0x44</t>
+  </si>
+  <si>
+    <t>Command</t>
+  </si>
+  <si>
+    <t>Move</t>
+  </si>
+  <si>
+    <t>move forward</t>
+  </si>
+  <si>
+    <t>move backward</t>
+  </si>
+  <si>
+    <t>turn left</t>
+  </si>
+  <si>
+    <t>turn right</t>
+  </si>
+  <si>
+    <t>Start Command</t>
+  </si>
+  <si>
+    <t>Byte:</t>
+  </si>
+  <si>
+    <t>MOVEMENT</t>
+  </si>
+  <si>
+    <t>IR DATA</t>
+  </si>
+  <si>
+    <t>right IR</t>
+  </si>
+  <si>
+    <t>left IR</t>
+  </si>
+  <si>
+    <t>back IR</t>
+  </si>
+  <si>
+    <t>0x01</t>
+  </si>
+  <si>
+    <t>0x02</t>
+  </si>
+  <si>
+    <t>0x03</t>
+  </si>
+  <si>
+    <t>0x04</t>
+  </si>
+  <si>
+    <t>0x11</t>
+  </si>
+  <si>
+    <t>0x12</t>
+  </si>
+  <si>
+    <t>0x13</t>
+  </si>
+  <si>
+    <t>0x05</t>
+  </si>
+  <si>
+    <t>0x06</t>
+  </si>
+  <si>
+    <t>0x07</t>
+  </si>
+  <si>
+    <t>0x08</t>
+  </si>
+  <si>
+    <t>0x00</t>
+  </si>
+  <si>
+    <t>0x09</t>
+  </si>
+  <si>
+    <t>0x0A</t>
+  </si>
+  <si>
+    <t>0x0B</t>
+  </si>
+  <si>
+    <t>0x0C</t>
+  </si>
+  <si>
+    <t>0x0D</t>
+  </si>
+  <si>
+    <t>0x0E</t>
+  </si>
+  <si>
+    <t>0x0F</t>
+  </si>
+  <si>
+    <t>Direction</t>
+  </si>
+  <si>
+    <t>Distance (Ticks)</t>
+  </si>
+  <si>
+    <t>Device Transmit</t>
+  </si>
+  <si>
+    <t>Pi</t>
+  </si>
+  <si>
+    <t>Tiva</t>
+  </si>
+  <si>
+    <t>2 Bytes of Data (max = 65535)</t>
+  </si>
+  <si>
+    <t>Send IR Value</t>
   </si>
 </sst>
 </file>
@@ -217,7 +335,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -225,11 +343,134 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -253,6 +494,40 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,11 +841,1025 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85CA0D59-C129-4927-BBCA-0FC73B637AB1}">
+  <dimension ref="A1:BJ51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z7" sqref="Z7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="9"/>
+    <col min="2" max="2" width="15.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="9"/>
+    <col min="4" max="4" width="14.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="12" width="2.77734375" style="14" customWidth="1"/>
+    <col min="13" max="13" width="6.6640625" style="12" customWidth="1"/>
+    <col min="14" max="21" width="2.77734375" style="9" customWidth="1"/>
+    <col min="22" max="22" width="6.6640625" style="1" customWidth="1"/>
+    <col min="23" max="54" width="2.77734375" style="9" customWidth="1"/>
+    <col min="55" max="55" width="13.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="56" max="16384" width="8.88671875" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="C1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="1">
+        <v>1</v>
+      </c>
+      <c r="E1" s="11">
+        <v>2</v>
+      </c>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="N1" s="10">
+        <v>3</v>
+      </c>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="W1" s="10">
+        <v>4</v>
+      </c>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="10"/>
+      <c r="AA1" s="10"/>
+      <c r="AB1" s="10"/>
+      <c r="AC1" s="10"/>
+      <c r="AD1" s="10"/>
+      <c r="AE1" s="10">
+        <v>5</v>
+      </c>
+      <c r="AF1" s="10"/>
+      <c r="AG1" s="10"/>
+      <c r="AH1" s="10"/>
+      <c r="AI1" s="10"/>
+      <c r="AJ1" s="10"/>
+      <c r="AK1" s="10"/>
+      <c r="AL1" s="10"/>
+      <c r="AM1" s="10">
+        <v>6</v>
+      </c>
+      <c r="AN1" s="10"/>
+      <c r="AO1" s="10"/>
+      <c r="AP1" s="10"/>
+      <c r="AQ1" s="10"/>
+      <c r="AR1" s="10"/>
+      <c r="AS1" s="10"/>
+      <c r="AT1" s="10"/>
+      <c r="AU1" s="10">
+        <v>7</v>
+      </c>
+      <c r="AV1" s="10"/>
+      <c r="AW1" s="10"/>
+      <c r="AX1" s="10"/>
+      <c r="AY1" s="10"/>
+      <c r="AZ1" s="10"/>
+      <c r="BA1" s="10"/>
+      <c r="BB1" s="10"/>
+      <c r="BC1" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="BC2" s="9" t="str">
+        <f t="shared" ref="BC2:BC51" si="0">IF($D2 = "Start Command", "End Command", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="BC3" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="B4" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="24"/>
+      <c r="BC4" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="15">
+        <v>0</v>
+      </c>
+      <c r="F5" s="16">
+        <v>0</v>
+      </c>
+      <c r="G5" s="16">
+        <v>0</v>
+      </c>
+      <c r="H5" s="16">
+        <v>0</v>
+      </c>
+      <c r="I5" s="16">
+        <v>0</v>
+      </c>
+      <c r="J5" s="16">
+        <v>0</v>
+      </c>
+      <c r="K5" s="16">
+        <v>0</v>
+      </c>
+      <c r="L5" s="16">
+        <v>1</v>
+      </c>
+      <c r="M5" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="BC5" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>End Command</v>
+      </c>
+    </row>
+    <row r="6" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="13">
+        <v>0</v>
+      </c>
+      <c r="F6" s="14">
+        <v>0</v>
+      </c>
+      <c r="G6" s="14">
+        <v>0</v>
+      </c>
+      <c r="H6" s="14">
+        <v>0</v>
+      </c>
+      <c r="I6" s="14">
+        <v>0</v>
+      </c>
+      <c r="J6" s="14">
+        <v>0</v>
+      </c>
+      <c r="K6" s="14">
+        <v>1</v>
+      </c>
+      <c r="L6" s="14">
+        <v>0</v>
+      </c>
+      <c r="M6" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="BC6" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>End Command</v>
+      </c>
+    </row>
+    <row r="7" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="13">
+        <v>0</v>
+      </c>
+      <c r="F7" s="14">
+        <v>0</v>
+      </c>
+      <c r="G7" s="14">
+        <v>0</v>
+      </c>
+      <c r="H7" s="14">
+        <v>0</v>
+      </c>
+      <c r="I7" s="14">
+        <v>0</v>
+      </c>
+      <c r="J7" s="14">
+        <v>0</v>
+      </c>
+      <c r="K7" s="14">
+        <v>1</v>
+      </c>
+      <c r="L7" s="14">
+        <v>1</v>
+      </c>
+      <c r="M7" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="N7" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="BC7" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>End Command</v>
+      </c>
+    </row>
+    <row r="8" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="19">
+        <v>0</v>
+      </c>
+      <c r="F8" s="20">
+        <v>0</v>
+      </c>
+      <c r="G8" s="20">
+        <v>0</v>
+      </c>
+      <c r="H8" s="20">
+        <v>0</v>
+      </c>
+      <c r="I8" s="20">
+        <v>0</v>
+      </c>
+      <c r="J8" s="20">
+        <v>1</v>
+      </c>
+      <c r="K8" s="20">
+        <v>0</v>
+      </c>
+      <c r="L8" s="20">
+        <v>0</v>
+      </c>
+      <c r="M8" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="N8" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="BC8" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>End Command</v>
+      </c>
+    </row>
+    <row r="9" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="BC9" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="B10" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="24"/>
+      <c r="BC10" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="15">
+        <v>0</v>
+      </c>
+      <c r="F11" s="16">
+        <v>0</v>
+      </c>
+      <c r="G11" s="16">
+        <v>0</v>
+      </c>
+      <c r="H11" s="16">
+        <v>1</v>
+      </c>
+      <c r="I11" s="16">
+        <v>0</v>
+      </c>
+      <c r="J11" s="16">
+        <v>0</v>
+      </c>
+      <c r="K11" s="16">
+        <v>0</v>
+      </c>
+      <c r="L11" s="16">
+        <v>1</v>
+      </c>
+      <c r="M11" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="BC11" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>End Command</v>
+      </c>
+    </row>
+    <row r="12" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="13">
+        <v>0</v>
+      </c>
+      <c r="F12" s="14">
+        <v>0</v>
+      </c>
+      <c r="G12" s="14">
+        <v>0</v>
+      </c>
+      <c r="H12" s="14">
+        <v>1</v>
+      </c>
+      <c r="I12" s="14">
+        <v>0</v>
+      </c>
+      <c r="J12" s="14">
+        <v>0</v>
+      </c>
+      <c r="K12" s="14">
+        <v>1</v>
+      </c>
+      <c r="L12" s="14">
+        <v>0</v>
+      </c>
+      <c r="M12" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="BC12" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>End Command</v>
+      </c>
+    </row>
+    <row r="13" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="19">
+        <v>0</v>
+      </c>
+      <c r="F13" s="20">
+        <v>0</v>
+      </c>
+      <c r="G13" s="20">
+        <v>0</v>
+      </c>
+      <c r="H13" s="20">
+        <v>1</v>
+      </c>
+      <c r="I13" s="20">
+        <v>0</v>
+      </c>
+      <c r="J13" s="20">
+        <v>0</v>
+      </c>
+      <c r="K13" s="20">
+        <v>1</v>
+      </c>
+      <c r="L13" s="20">
+        <v>1</v>
+      </c>
+      <c r="M13" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="BC13" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>End Command</v>
+      </c>
+    </row>
+    <row r="14" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="BC14" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="23"/>
+      <c r="Q15" s="23"/>
+      <c r="R15" s="23"/>
+      <c r="S15" s="23"/>
+      <c r="T15" s="23"/>
+      <c r="U15" s="23"/>
+      <c r="V15" s="24"/>
+      <c r="BC15" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>End Command</v>
+      </c>
+    </row>
+    <row r="16" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="BC16" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="7:55" x14ac:dyDescent="0.3">
+      <c r="BC17" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="7:55" x14ac:dyDescent="0.3">
+      <c r="BC18" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="7:55" x14ac:dyDescent="0.3">
+      <c r="BC19" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="7:55" x14ac:dyDescent="0.3">
+      <c r="BC20" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="7:55" x14ac:dyDescent="0.3">
+      <c r="G21" s="14">
+        <v>0</v>
+      </c>
+      <c r="H21" s="14">
+        <v>0</v>
+      </c>
+      <c r="I21" s="14">
+        <v>0</v>
+      </c>
+      <c r="J21" s="14">
+        <v>0</v>
+      </c>
+      <c r="M21" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="BC21" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="7:55" x14ac:dyDescent="0.3">
+      <c r="G22" s="14">
+        <v>0</v>
+      </c>
+      <c r="H22" s="14">
+        <v>0</v>
+      </c>
+      <c r="I22" s="14">
+        <v>0</v>
+      </c>
+      <c r="J22" s="14">
+        <v>1</v>
+      </c>
+      <c r="M22" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="BC22" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="7:55" x14ac:dyDescent="0.3">
+      <c r="G23" s="14">
+        <v>0</v>
+      </c>
+      <c r="H23" s="14">
+        <v>0</v>
+      </c>
+      <c r="I23" s="14">
+        <v>1</v>
+      </c>
+      <c r="J23" s="14">
+        <v>0</v>
+      </c>
+      <c r="M23" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="BC23" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="7:55" x14ac:dyDescent="0.3">
+      <c r="G24" s="14">
+        <v>0</v>
+      </c>
+      <c r="H24" s="14">
+        <v>0</v>
+      </c>
+      <c r="I24" s="14">
+        <v>1</v>
+      </c>
+      <c r="J24" s="14">
+        <v>1</v>
+      </c>
+      <c r="M24" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="BC24" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="7:55" x14ac:dyDescent="0.3">
+      <c r="G25" s="14">
+        <v>0</v>
+      </c>
+      <c r="H25" s="14">
+        <v>1</v>
+      </c>
+      <c r="I25" s="14">
+        <v>0</v>
+      </c>
+      <c r="J25" s="14">
+        <v>0</v>
+      </c>
+      <c r="M25" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="BC25" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="7:55" x14ac:dyDescent="0.3">
+      <c r="G26" s="14">
+        <v>0</v>
+      </c>
+      <c r="H26" s="14">
+        <v>1</v>
+      </c>
+      <c r="I26" s="14">
+        <v>0</v>
+      </c>
+      <c r="J26" s="14">
+        <v>1</v>
+      </c>
+      <c r="M26" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="BC26" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="7:55" x14ac:dyDescent="0.3">
+      <c r="G27" s="14">
+        <v>0</v>
+      </c>
+      <c r="H27" s="14">
+        <v>1</v>
+      </c>
+      <c r="I27" s="14">
+        <v>1</v>
+      </c>
+      <c r="J27" s="14">
+        <v>0</v>
+      </c>
+      <c r="M27" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="BC27" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="7:55" x14ac:dyDescent="0.3">
+      <c r="G28" s="14">
+        <v>0</v>
+      </c>
+      <c r="H28" s="14">
+        <v>1</v>
+      </c>
+      <c r="I28" s="14">
+        <v>1</v>
+      </c>
+      <c r="J28" s="14">
+        <v>1</v>
+      </c>
+      <c r="M28" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="BC28" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="7:55" x14ac:dyDescent="0.3">
+      <c r="G29" s="14">
+        <v>1</v>
+      </c>
+      <c r="H29" s="14">
+        <v>0</v>
+      </c>
+      <c r="I29" s="14">
+        <v>0</v>
+      </c>
+      <c r="J29" s="14">
+        <v>0</v>
+      </c>
+      <c r="M29" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="BC29" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="7:55" x14ac:dyDescent="0.3">
+      <c r="G30" s="14">
+        <v>1</v>
+      </c>
+      <c r="H30" s="14">
+        <v>0</v>
+      </c>
+      <c r="I30" s="14">
+        <v>0</v>
+      </c>
+      <c r="J30" s="14">
+        <v>1</v>
+      </c>
+      <c r="M30" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="BC30" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="7:55" x14ac:dyDescent="0.3">
+      <c r="G31" s="14">
+        <v>1</v>
+      </c>
+      <c r="H31" s="14">
+        <v>0</v>
+      </c>
+      <c r="I31" s="14">
+        <v>1</v>
+      </c>
+      <c r="J31" s="14">
+        <v>0</v>
+      </c>
+      <c r="M31" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="BC31" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="7:55" x14ac:dyDescent="0.3">
+      <c r="G32" s="14">
+        <v>1</v>
+      </c>
+      <c r="H32" s="14">
+        <v>0</v>
+      </c>
+      <c r="I32" s="14">
+        <v>1</v>
+      </c>
+      <c r="J32" s="14">
+        <v>1</v>
+      </c>
+      <c r="M32" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="BC32" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="7:55" x14ac:dyDescent="0.3">
+      <c r="G33" s="14">
+        <v>1</v>
+      </c>
+      <c r="H33" s="14">
+        <v>1</v>
+      </c>
+      <c r="I33" s="14">
+        <v>0</v>
+      </c>
+      <c r="J33" s="14">
+        <v>0</v>
+      </c>
+      <c r="M33" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="BC33" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="7:55" x14ac:dyDescent="0.3">
+      <c r="G34" s="14">
+        <v>1</v>
+      </c>
+      <c r="H34" s="14">
+        <v>1</v>
+      </c>
+      <c r="I34" s="14">
+        <v>0</v>
+      </c>
+      <c r="J34" s="14">
+        <v>1</v>
+      </c>
+      <c r="M34" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="BC34" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="7:55" x14ac:dyDescent="0.3">
+      <c r="G35" s="14">
+        <v>1</v>
+      </c>
+      <c r="H35" s="14">
+        <v>1</v>
+      </c>
+      <c r="I35" s="14">
+        <v>1</v>
+      </c>
+      <c r="J35" s="14">
+        <v>0</v>
+      </c>
+      <c r="M35" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="BC35" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="7:55" x14ac:dyDescent="0.3">
+      <c r="G36" s="14">
+        <v>1</v>
+      </c>
+      <c r="H36" s="14">
+        <v>1</v>
+      </c>
+      <c r="I36" s="14">
+        <v>1</v>
+      </c>
+      <c r="J36" s="14">
+        <v>1</v>
+      </c>
+      <c r="M36" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="BC36" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="7:55" x14ac:dyDescent="0.3">
+      <c r="BC37" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="7:55" x14ac:dyDescent="0.3">
+      <c r="BC38" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="7:55" x14ac:dyDescent="0.3">
+      <c r="BC39" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="7:55" x14ac:dyDescent="0.3">
+      <c r="BC40" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="7:55" x14ac:dyDescent="0.3">
+      <c r="BC41" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="7:55" x14ac:dyDescent="0.3">
+      <c r="BC42" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="7:55" x14ac:dyDescent="0.3">
+      <c r="BC43" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="7:55" x14ac:dyDescent="0.3">
+      <c r="BC44" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="7:55" x14ac:dyDescent="0.3">
+      <c r="BC45" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="7:55" x14ac:dyDescent="0.3">
+      <c r="BC46" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="7:55" x14ac:dyDescent="0.3">
+      <c r="BC47" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="7:55" x14ac:dyDescent="0.3">
+      <c r="BC48" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="55:55" x14ac:dyDescent="0.3">
+      <c r="BC49" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="55:55" x14ac:dyDescent="0.3">
+      <c r="BC50" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="55:55" x14ac:dyDescent="0.3">
+      <c r="BC51" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="E15:V15"/>
+    <mergeCell ref="AU1:BB1"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="E10:H10"/>
+    <mergeCell ref="N5:U5"/>
+    <mergeCell ref="N6:U6"/>
+    <mergeCell ref="N7:U7"/>
+    <mergeCell ref="N8:U8"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="E1:L1"/>
+    <mergeCell ref="N1:U1"/>
+    <mergeCell ref="W1:AD1"/>
+    <mergeCell ref="AE1:AL1"/>
+    <mergeCell ref="AM1:AT1"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6836315B-2C81-4F83-8718-E67FA02C11DA}">
   <dimension ref="A1:AD40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P29" sqref="P29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
moved all of lab_6 main into a function in trans_receiver. created lab7 main in preparation for obstacle avoidance. updated packet protocol with command for navigating to xy coordinates.
</commit_message>
<xml_diff>
--- a/Command_Data Planner.xlsx
+++ b/Command_Data Planner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emily\bishop_ecpe155_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77B9791-BC14-4528-956E-522DC2B836A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B14879C-D814-4B25-AB6F-B908E92C658F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{41C8675F-361B-4635-AFD0-4B5E8933C9D2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="81">
   <si>
     <t xml:space="preserve">command </t>
   </si>
@@ -270,6 +270,15 @@
   </si>
   <si>
     <t>Distance (cm)</t>
+  </si>
+  <si>
+    <t>navigate to XY</t>
+  </si>
+  <si>
+    <t>Distance X (cm)</t>
+  </si>
+  <si>
+    <t>Distance Y (cm)</t>
   </si>
 </sst>
 </file>
@@ -335,7 +344,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -466,11 +475,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -519,6 +548,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -531,6 +563,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -845,10 +879,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85CA0D59-C129-4927-BBCA-0FC73B637AB1}">
-  <dimension ref="A1:BC51"/>
+  <dimension ref="A1:BC52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W8" sqref="W8:AD8"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="W10" sqref="W10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -873,66 +907,66 @@
       <c r="D1" s="1">
         <v>1</v>
       </c>
-      <c r="E1" s="25">
+      <c r="E1" s="26">
         <v>2</v>
       </c>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="N1" s="21">
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="N1" s="22">
         <v>3</v>
       </c>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="21"/>
-      <c r="U1" s="21"/>
-      <c r="W1" s="21">
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="W1" s="22">
         <v>4</v>
       </c>
-      <c r="X1" s="21"/>
-      <c r="Y1" s="21"/>
-      <c r="Z1" s="21"/>
-      <c r="AA1" s="21"/>
-      <c r="AB1" s="21"/>
-      <c r="AC1" s="21"/>
-      <c r="AD1" s="21"/>
-      <c r="AE1" s="21">
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="22"/>
+      <c r="AD1" s="22"/>
+      <c r="AE1" s="22">
         <v>5</v>
       </c>
-      <c r="AF1" s="21"/>
-      <c r="AG1" s="21"/>
-      <c r="AH1" s="21"/>
-      <c r="AI1" s="21"/>
-      <c r="AJ1" s="21"/>
-      <c r="AK1" s="21"/>
-      <c r="AL1" s="21"/>
-      <c r="AM1" s="21">
+      <c r="AF1" s="22"/>
+      <c r="AG1" s="22"/>
+      <c r="AH1" s="22"/>
+      <c r="AI1" s="22"/>
+      <c r="AJ1" s="22"/>
+      <c r="AK1" s="22"/>
+      <c r="AL1" s="22"/>
+      <c r="AM1" s="22">
         <v>6</v>
       </c>
-      <c r="AN1" s="21"/>
-      <c r="AO1" s="21"/>
-      <c r="AP1" s="21"/>
-      <c r="AQ1" s="21"/>
-      <c r="AR1" s="21"/>
-      <c r="AS1" s="21"/>
-      <c r="AT1" s="21"/>
-      <c r="AU1" s="21">
+      <c r="AN1" s="22"/>
+      <c r="AO1" s="22"/>
+      <c r="AP1" s="22"/>
+      <c r="AQ1" s="22"/>
+      <c r="AR1" s="22"/>
+      <c r="AS1" s="22"/>
+      <c r="AT1" s="22"/>
+      <c r="AU1" s="22">
         <v>7</v>
       </c>
-      <c r="AV1" s="21"/>
-      <c r="AW1" s="21"/>
-      <c r="AX1" s="21"/>
-      <c r="AY1" s="21"/>
-      <c r="AZ1" s="21"/>
-      <c r="BA1" s="21"/>
-      <c r="BB1" s="21"/>
+      <c r="AV1" s="22"/>
+      <c r="AW1" s="22"/>
+      <c r="AX1" s="22"/>
+      <c r="AY1" s="22"/>
+      <c r="AZ1" s="22"/>
+      <c r="BA1" s="22"/>
+      <c r="BB1" s="22"/>
       <c r="BC1" s="1">
         <v>8</v>
       </c>
@@ -945,7 +979,7 @@
         <v>39</v>
       </c>
       <c r="BC2" s="9" t="str">
-        <f t="shared" ref="BC2:BC51" si="0">IF($D2 = "Start Command", "End Command", "")</f>
+        <f t="shared" ref="BC2:BC52" si="0">IF($D2 = "Start Command", "End Command", "")</f>
         <v/>
       </c>
     </row>
@@ -959,18 +993,18 @@
       <c r="B4" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="22" t="s">
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="25"/>
       <c r="BC4" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1013,24 +1047,24 @@
       <c r="M5" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="N5" s="21" t="s">
+      <c r="N5" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="21"/>
-      <c r="S5" s="21"/>
-      <c r="T5" s="21"/>
-      <c r="U5" s="21"/>
-      <c r="W5" s="21"/>
-      <c r="X5" s="21"/>
-      <c r="Y5" s="21"/>
-      <c r="Z5" s="21"/>
-      <c r="AA5" s="21"/>
-      <c r="AB5" s="21"/>
-      <c r="AC5" s="21"/>
-      <c r="AD5" s="21"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="22"/>
+      <c r="S5" s="22"/>
+      <c r="T5" s="22"/>
+      <c r="U5" s="22"/>
+      <c r="W5" s="22"/>
+      <c r="X5" s="22"/>
+      <c r="Y5" s="22"/>
+      <c r="Z5" s="22"/>
+      <c r="AA5" s="22"/>
+      <c r="AB5" s="22"/>
+      <c r="AC5" s="22"/>
+      <c r="AD5" s="22"/>
       <c r="BC5" s="9" t="str">
         <f t="shared" si="0"/>
         <v>End Command</v>
@@ -1073,24 +1107,24 @@
       <c r="M6" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="N6" s="21" t="s">
+      <c r="N6" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="O6" s="21"/>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="21"/>
-      <c r="R6" s="21"/>
-      <c r="S6" s="21"/>
-      <c r="T6" s="21"/>
-      <c r="U6" s="21"/>
-      <c r="W6" s="21"/>
-      <c r="X6" s="21"/>
-      <c r="Y6" s="21"/>
-      <c r="Z6" s="21"/>
-      <c r="AA6" s="21"/>
-      <c r="AB6" s="21"/>
-      <c r="AC6" s="21"/>
-      <c r="AD6" s="21"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="22"/>
+      <c r="R6" s="22"/>
+      <c r="S6" s="22"/>
+      <c r="T6" s="22"/>
+      <c r="U6" s="22"/>
+      <c r="W6" s="22"/>
+      <c r="X6" s="22"/>
+      <c r="Y6" s="22"/>
+      <c r="Z6" s="22"/>
+      <c r="AA6" s="22"/>
+      <c r="AB6" s="22"/>
+      <c r="AC6" s="22"/>
+      <c r="AD6" s="22"/>
       <c r="BC6" s="9" t="str">
         <f t="shared" si="0"/>
         <v>End Command</v>
@@ -1133,23 +1167,23 @@
       <c r="M7" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="21"/>
-      <c r="S7" s="21"/>
-      <c r="T7" s="21"/>
-      <c r="U7" s="21"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="22"/>
+      <c r="S7" s="22"/>
+      <c r="T7" s="22"/>
+      <c r="U7" s="22"/>
       <c r="V7" s="10"/>
-      <c r="W7" s="21"/>
-      <c r="X7" s="21"/>
-      <c r="Y7" s="21"/>
-      <c r="Z7" s="21"/>
-      <c r="AA7" s="21"/>
-      <c r="AB7" s="21"/>
-      <c r="AC7" s="21"/>
-      <c r="AD7" s="21"/>
+      <c r="W7" s="22"/>
+      <c r="X7" s="22"/>
+      <c r="Y7" s="22"/>
+      <c r="Z7" s="22"/>
+      <c r="AA7" s="22"/>
+      <c r="AB7" s="22"/>
+      <c r="AC7" s="22"/>
+      <c r="AD7" s="22"/>
       <c r="BC7" s="9" t="str">
         <f t="shared" si="0"/>
         <v>End Command</v>
@@ -1165,122 +1199,143 @@
       <c r="D8" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="18">
-        <v>0</v>
-      </c>
-      <c r="F8" s="19">
-        <v>0</v>
-      </c>
-      <c r="G8" s="19">
-        <v>0</v>
-      </c>
-      <c r="H8" s="19">
-        <v>0</v>
-      </c>
-      <c r="I8" s="19">
-        <v>0</v>
-      </c>
-      <c r="J8" s="19">
-        <v>1</v>
-      </c>
-      <c r="K8" s="19">
-        <v>0</v>
-      </c>
-      <c r="L8" s="19">
-        <v>0</v>
-      </c>
-      <c r="M8" s="20" t="s">
+      <c r="E8" s="12">
+        <v>0</v>
+      </c>
+      <c r="F8" s="13">
+        <v>0</v>
+      </c>
+      <c r="G8" s="13">
+        <v>0</v>
+      </c>
+      <c r="H8" s="13">
+        <v>0</v>
+      </c>
+      <c r="I8" s="13">
+        <v>0</v>
+      </c>
+      <c r="J8" s="13">
+        <v>1</v>
+      </c>
+      <c r="K8" s="13">
+        <v>0</v>
+      </c>
+      <c r="L8" s="28">
+        <v>0</v>
+      </c>
+      <c r="M8" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="N8" s="21"/>
-      <c r="O8" s="21"/>
-      <c r="P8" s="21"/>
-      <c r="Q8" s="21"/>
-      <c r="R8" s="21"/>
-      <c r="S8" s="21"/>
-      <c r="T8" s="21"/>
-      <c r="U8" s="21"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="22"/>
+      <c r="P8" s="22"/>
+      <c r="Q8" s="22"/>
+      <c r="R8" s="22"/>
+      <c r="S8" s="22"/>
+      <c r="T8" s="22"/>
+      <c r="U8" s="22"/>
       <c r="V8" s="10"/>
-      <c r="W8" s="21"/>
-      <c r="X8" s="21"/>
-      <c r="Y8" s="21"/>
-      <c r="Z8" s="21"/>
-      <c r="AA8" s="21"/>
-      <c r="AB8" s="21"/>
-      <c r="AC8" s="21"/>
-      <c r="AD8" s="21"/>
+      <c r="W8" s="22"/>
+      <c r="X8" s="22"/>
+      <c r="Y8" s="22"/>
+      <c r="Z8" s="22"/>
+      <c r="AA8" s="22"/>
+      <c r="AB8" s="22"/>
+      <c r="AC8" s="22"/>
+      <c r="AD8" s="22"/>
       <c r="BC8" s="9" t="str">
         <f t="shared" si="0"/>
         <v>End Command</v>
       </c>
     </row>
     <row r="9" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="18">
+        <v>0</v>
+      </c>
+      <c r="F9" s="19">
+        <v>0</v>
+      </c>
+      <c r="G9" s="19">
+        <v>0</v>
+      </c>
+      <c r="H9" s="19">
+        <v>0</v>
+      </c>
+      <c r="I9" s="19">
+        <v>0</v>
+      </c>
+      <c r="J9" s="19">
+        <v>1</v>
+      </c>
+      <c r="K9" s="19">
+        <v>0</v>
+      </c>
+      <c r="L9" s="27">
+        <v>1</v>
+      </c>
+      <c r="M9" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="N9" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="22"/>
+      <c r="S9" s="22"/>
+      <c r="T9" s="22"/>
+      <c r="U9" s="22"/>
+      <c r="V9" s="21"/>
+      <c r="W9" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="X9" s="22"/>
+      <c r="Y9" s="22"/>
+      <c r="Z9" s="22"/>
+      <c r="AA9" s="22"/>
+      <c r="AB9" s="22"/>
+      <c r="AC9" s="22"/>
+      <c r="AD9" s="22"/>
       <c r="BC9" s="9" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>End Command</v>
       </c>
     </row>
     <row r="10" spans="1:55" x14ac:dyDescent="0.3">
-      <c r="B10" s="9" t="s">
+      <c r="BC10" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="B11" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E11" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="22" t="s">
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="24"/>
-      <c r="BC10" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:55" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="14">
-        <v>0</v>
-      </c>
-      <c r="F11" s="15">
-        <v>0</v>
-      </c>
-      <c r="G11" s="15">
-        <v>0</v>
-      </c>
-      <c r="H11" s="15">
-        <v>1</v>
-      </c>
-      <c r="I11" s="15">
-        <v>0</v>
-      </c>
-      <c r="J11" s="15">
-        <v>0</v>
-      </c>
-      <c r="K11" s="15">
-        <v>0</v>
-      </c>
-      <c r="L11" s="15">
-        <v>1</v>
-      </c>
-      <c r="M11" s="16" t="s">
-        <v>56</v>
-      </c>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="25"/>
       <c r="BC11" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>End Command</v>
+        <v/>
       </c>
     </row>
     <row r="12" spans="1:55" x14ac:dyDescent="0.3">
@@ -1288,37 +1343,37 @@
         <v>73</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="12">
-        <v>0</v>
-      </c>
-      <c r="F12" s="13">
-        <v>0</v>
-      </c>
-      <c r="G12" s="13">
-        <v>0</v>
-      </c>
-      <c r="H12" s="13">
-        <v>1</v>
-      </c>
-      <c r="I12" s="13">
-        <v>0</v>
-      </c>
-      <c r="J12" s="13">
-        <v>0</v>
-      </c>
-      <c r="K12" s="13">
-        <v>1</v>
-      </c>
-      <c r="L12" s="13">
-        <v>0</v>
-      </c>
-      <c r="M12" s="17" t="s">
-        <v>57</v>
+      <c r="E12" s="14">
+        <v>0</v>
+      </c>
+      <c r="F12" s="15">
+        <v>0</v>
+      </c>
+      <c r="G12" s="15">
+        <v>0</v>
+      </c>
+      <c r="H12" s="15">
+        <v>1</v>
+      </c>
+      <c r="I12" s="15">
+        <v>0</v>
+      </c>
+      <c r="J12" s="15">
+        <v>0</v>
+      </c>
+      <c r="K12" s="15">
+        <v>0</v>
+      </c>
+      <c r="L12" s="15">
+        <v>1</v>
+      </c>
+      <c r="M12" s="16" t="s">
+        <v>56</v>
       </c>
       <c r="BC12" s="9" t="str">
         <f t="shared" si="0"/>
@@ -1330,88 +1385,124 @@
         <v>73</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="18">
-        <v>0</v>
-      </c>
-      <c r="F13" s="19">
-        <v>0</v>
-      </c>
-      <c r="G13" s="19">
-        <v>0</v>
-      </c>
-      <c r="H13" s="19">
-        <v>1</v>
-      </c>
-      <c r="I13" s="19">
-        <v>0</v>
-      </c>
-      <c r="J13" s="19">
-        <v>0</v>
-      </c>
-      <c r="K13" s="19">
-        <v>1</v>
-      </c>
-      <c r="L13" s="19">
-        <v>1</v>
-      </c>
-      <c r="M13" s="20" t="s">
+      <c r="E13" s="12">
+        <v>0</v>
+      </c>
+      <c r="F13" s="13">
+        <v>0</v>
+      </c>
+      <c r="G13" s="13">
+        <v>0</v>
+      </c>
+      <c r="H13" s="13">
+        <v>1</v>
+      </c>
+      <c r="I13" s="13">
+        <v>0</v>
+      </c>
+      <c r="J13" s="13">
+        <v>0</v>
+      </c>
+      <c r="K13" s="13">
+        <v>1</v>
+      </c>
+      <c r="L13" s="13">
+        <v>0</v>
+      </c>
+      <c r="M13" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="BC13" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>End Command</v>
+      </c>
+    </row>
+    <row r="14" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="18">
+        <v>0</v>
+      </c>
+      <c r="F14" s="19">
+        <v>0</v>
+      </c>
+      <c r="G14" s="19">
+        <v>0</v>
+      </c>
+      <c r="H14" s="19">
+        <v>1</v>
+      </c>
+      <c r="I14" s="19">
+        <v>0</v>
+      </c>
+      <c r="J14" s="19">
+        <v>0</v>
+      </c>
+      <c r="K14" s="19">
+        <v>1</v>
+      </c>
+      <c r="L14" s="19">
+        <v>1</v>
+      </c>
+      <c r="M14" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="BC13" s="9" t="str">
+      <c r="BC14" s="9" t="str">
         <f t="shared" si="0"/>
         <v>End Command</v>
       </c>
     </row>
-    <row r="14" spans="1:55" x14ac:dyDescent="0.3">
-      <c r="BC14" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
     <row r="15" spans="1:55" x14ac:dyDescent="0.3">
-      <c r="A15" s="9" t="s">
+      <c r="BC15" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B16" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D16" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="E16" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="23"/>
-      <c r="M15" s="23"/>
-      <c r="N15" s="23"/>
-      <c r="O15" s="23"/>
-      <c r="P15" s="23"/>
-      <c r="Q15" s="23"/>
-      <c r="R15" s="23"/>
-      <c r="S15" s="23"/>
-      <c r="T15" s="23"/>
-      <c r="U15" s="23"/>
-      <c r="V15" s="24"/>
-      <c r="BC15" s="9" t="str">
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="24"/>
+      <c r="N16" s="24"/>
+      <c r="O16" s="24"/>
+      <c r="P16" s="24"/>
+      <c r="Q16" s="24"/>
+      <c r="R16" s="24"/>
+      <c r="S16" s="24"/>
+      <c r="T16" s="24"/>
+      <c r="U16" s="24"/>
+      <c r="V16" s="25"/>
+      <c r="BC16" s="9" t="str">
         <f t="shared" si="0"/>
         <v>End Command</v>
-      </c>
-    </row>
-    <row r="16" spans="1:55" x14ac:dyDescent="0.3">
-      <c r="BC16" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
       </c>
     </row>
     <row r="17" spans="7:55" x14ac:dyDescent="0.3">
@@ -1439,21 +1530,6 @@
       </c>
     </row>
     <row r="21" spans="7:55" x14ac:dyDescent="0.3">
-      <c r="G21" s="13">
-        <v>0</v>
-      </c>
-      <c r="H21" s="13">
-        <v>0</v>
-      </c>
-      <c r="I21" s="13">
-        <v>0</v>
-      </c>
-      <c r="J21" s="13">
-        <v>0</v>
-      </c>
-      <c r="M21" s="11" t="s">
-        <v>63</v>
-      </c>
       <c r="BC21" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1470,10 +1546,10 @@
         <v>0</v>
       </c>
       <c r="J22" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M22" s="11" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="BC22" s="9" t="str">
         <f t="shared" si="0"/>
@@ -1488,13 +1564,13 @@
         <v>0</v>
       </c>
       <c r="I23" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M23" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="BC23" s="9" t="str">
         <f t="shared" si="0"/>
@@ -1512,10 +1588,10 @@
         <v>1</v>
       </c>
       <c r="J24" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M24" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="BC24" s="9" t="str">
         <f t="shared" si="0"/>
@@ -1527,16 +1603,16 @@
         <v>0</v>
       </c>
       <c r="H25" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M25" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="BC25" s="9" t="str">
         <f t="shared" si="0"/>
@@ -1554,10 +1630,10 @@
         <v>0</v>
       </c>
       <c r="J26" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M26" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="BC26" s="9" t="str">
         <f t="shared" si="0"/>
@@ -1572,13 +1648,13 @@
         <v>1</v>
       </c>
       <c r="I27" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M27" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="BC27" s="9" t="str">
         <f t="shared" si="0"/>
@@ -1596,10 +1672,10 @@
         <v>1</v>
       </c>
       <c r="J28" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M28" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="BC28" s="9" t="str">
         <f t="shared" si="0"/>
@@ -1608,19 +1684,19 @@
     </row>
     <row r="29" spans="7:55" x14ac:dyDescent="0.3">
       <c r="G29" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H29" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M29" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="BC29" s="9" t="str">
         <f t="shared" si="0"/>
@@ -1638,10 +1714,10 @@
         <v>0</v>
       </c>
       <c r="J30" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M30" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="BC30" s="9" t="str">
         <f t="shared" si="0"/>
@@ -1656,13 +1732,13 @@
         <v>0</v>
       </c>
       <c r="I31" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J31" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M31" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="BC31" s="9" t="str">
         <f t="shared" si="0"/>
@@ -1680,10 +1756,10 @@
         <v>1</v>
       </c>
       <c r="J32" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M32" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="BC32" s="9" t="str">
         <f t="shared" si="0"/>
@@ -1695,16 +1771,16 @@
         <v>1</v>
       </c>
       <c r="H33" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I33" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J33" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M33" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BC33" s="9" t="str">
         <f t="shared" si="0"/>
@@ -1722,10 +1798,10 @@
         <v>0</v>
       </c>
       <c r="J34" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M34" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="BC34" s="9" t="str">
         <f t="shared" si="0"/>
@@ -1740,13 +1816,13 @@
         <v>1</v>
       </c>
       <c r="I35" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J35" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M35" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BC35" s="9" t="str">
         <f t="shared" si="0"/>
@@ -1764,17 +1840,32 @@
         <v>1</v>
       </c>
       <c r="J36" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M36" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="BC36" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="7:55" x14ac:dyDescent="0.3">
+      <c r="G37" s="13">
+        <v>1</v>
+      </c>
+      <c r="H37" s="13">
+        <v>1</v>
+      </c>
+      <c r="I37" s="13">
+        <v>1</v>
+      </c>
+      <c r="J37" s="13">
+        <v>1</v>
+      </c>
+      <c r="M37" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="BC36" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="7:55" x14ac:dyDescent="0.3">
       <c r="BC37" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1864,27 +1955,35 @@
         <v/>
       </c>
     </row>
+    <row r="52" spans="55:55" x14ac:dyDescent="0.3">
+      <c r="BC52" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="21">
+    <mergeCell ref="W8:AD8"/>
+    <mergeCell ref="E16:V16"/>
+    <mergeCell ref="AU1:BB1"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="E11:H11"/>
+    <mergeCell ref="N5:U5"/>
+    <mergeCell ref="N6:U6"/>
+    <mergeCell ref="N7:U7"/>
+    <mergeCell ref="N8:U8"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="I11:L11"/>
+    <mergeCell ref="E1:L1"/>
+    <mergeCell ref="N1:U1"/>
+    <mergeCell ref="W1:AD1"/>
+    <mergeCell ref="N9:U9"/>
+    <mergeCell ref="W9:AD9"/>
     <mergeCell ref="AE1:AL1"/>
     <mergeCell ref="AM1:AT1"/>
     <mergeCell ref="W5:AD5"/>
     <mergeCell ref="W6:AD6"/>
     <mergeCell ref="W7:AD7"/>
-    <mergeCell ref="W8:AD8"/>
-    <mergeCell ref="E15:V15"/>
-    <mergeCell ref="AU1:BB1"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="E10:H10"/>
-    <mergeCell ref="N5:U5"/>
-    <mergeCell ref="N6:U6"/>
-    <mergeCell ref="N7:U7"/>
-    <mergeCell ref="N8:U8"/>
-    <mergeCell ref="I4:L4"/>
-    <mergeCell ref="I10:L10"/>
-    <mergeCell ref="E1:L1"/>
-    <mergeCell ref="N1:U1"/>
-    <mergeCell ref="W1:AD1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
More Additions to PID Code
</commit_message>
<xml_diff>
--- a/Command_Data Planner.xlsx
+++ b/Command_Data Planner.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emily\bishop_ecpe155_2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Materia\2022 Spring\Courses\ECPE-155 Autonomous Robotics\Labs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF4C5AF-CF1B-4CD7-9475-8260293422F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE56F7D-2707-4F73-8C50-9E78021543FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{41C8675F-361B-4635-AFD0-4B5E8933C9D2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{41C8675F-361B-4635-AFD0-4B5E8933C9D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Packet Protocol" sheetId="4" r:id="rId1"/>
@@ -254,9 +254,6 @@
     <t>Direction</t>
   </si>
   <si>
-    <t>Distance (Ticks)</t>
-  </si>
-  <si>
     <t>Device Transmit</t>
   </si>
   <si>
@@ -270,6 +267,9 @@
   </si>
   <si>
     <t>Send IR Value</t>
+  </si>
+  <si>
+    <t>Distance (cm)</t>
   </si>
 </sst>
 </file>
@@ -495,12 +495,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -526,6 +520,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -842,101 +842,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85CA0D59-C129-4927-BBCA-0FC73B637AB1}">
-  <dimension ref="A1:BJ51"/>
+  <dimension ref="A1:BC51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z7" sqref="Z7"/>
+      <selection activeCell="N8" sqref="N8:U8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="9"/>
-    <col min="2" max="2" width="15.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="9"/>
-    <col min="4" max="4" width="14.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="12" width="2.77734375" style="14" customWidth="1"/>
-    <col min="13" max="13" width="6.6640625" style="12" customWidth="1"/>
-    <col min="14" max="21" width="2.77734375" style="9" customWidth="1"/>
-    <col min="22" max="22" width="6.6640625" style="1" customWidth="1"/>
-    <col min="23" max="54" width="2.77734375" style="9" customWidth="1"/>
-    <col min="55" max="55" width="13.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="56" max="16384" width="8.88671875" style="9"/>
+    <col min="1" max="1" width="8.85546875" style="9"/>
+    <col min="2" max="2" width="15.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="9"/>
+    <col min="4" max="4" width="14.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="12" width="2.7109375" style="12" customWidth="1"/>
+    <col min="13" max="13" width="6.7109375" style="10" customWidth="1"/>
+    <col min="14" max="21" width="2.7109375" style="9" customWidth="1"/>
+    <col min="22" max="22" width="6.7109375" style="1" customWidth="1"/>
+    <col min="23" max="54" width="2.7109375" style="9" customWidth="1"/>
+    <col min="55" max="55" width="13.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="56" max="16384" width="8.85546875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:55" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
         <v>46</v>
       </c>
       <c r="D1" s="1">
         <v>1</v>
       </c>
-      <c r="E1" s="11">
+      <c r="E1" s="24">
         <v>2</v>
       </c>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="N1" s="10">
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="N1" s="23">
         <v>3</v>
       </c>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="W1" s="10">
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
+      <c r="W1" s="23">
         <v>4</v>
       </c>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
-      <c r="AA1" s="10"/>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="10"/>
-      <c r="AD1" s="10"/>
-      <c r="AE1" s="10">
+      <c r="X1" s="23"/>
+      <c r="Y1" s="23"/>
+      <c r="Z1" s="23"/>
+      <c r="AA1" s="23"/>
+      <c r="AB1" s="23"/>
+      <c r="AC1" s="23"/>
+      <c r="AD1" s="23"/>
+      <c r="AE1" s="23">
         <v>5</v>
       </c>
-      <c r="AF1" s="10"/>
-      <c r="AG1" s="10"/>
-      <c r="AH1" s="10"/>
-      <c r="AI1" s="10"/>
-      <c r="AJ1" s="10"/>
-      <c r="AK1" s="10"/>
-      <c r="AL1" s="10"/>
-      <c r="AM1" s="10">
+      <c r="AF1" s="23"/>
+      <c r="AG1" s="23"/>
+      <c r="AH1" s="23"/>
+      <c r="AI1" s="23"/>
+      <c r="AJ1" s="23"/>
+      <c r="AK1" s="23"/>
+      <c r="AL1" s="23"/>
+      <c r="AM1" s="23">
         <v>6</v>
       </c>
-      <c r="AN1" s="10"/>
-      <c r="AO1" s="10"/>
-      <c r="AP1" s="10"/>
-      <c r="AQ1" s="10"/>
-      <c r="AR1" s="10"/>
-      <c r="AS1" s="10"/>
-      <c r="AT1" s="10"/>
-      <c r="AU1" s="10">
+      <c r="AN1" s="23"/>
+      <c r="AO1" s="23"/>
+      <c r="AP1" s="23"/>
+      <c r="AQ1" s="23"/>
+      <c r="AR1" s="23"/>
+      <c r="AS1" s="23"/>
+      <c r="AT1" s="23"/>
+      <c r="AU1" s="23">
         <v>7</v>
       </c>
-      <c r="AV1" s="10"/>
-      <c r="AW1" s="10"/>
-      <c r="AX1" s="10"/>
-      <c r="AY1" s="10"/>
-      <c r="AZ1" s="10"/>
-      <c r="BA1" s="10"/>
-      <c r="BB1" s="10"/>
+      <c r="AV1" s="23"/>
+      <c r="AW1" s="23"/>
+      <c r="AX1" s="23"/>
+      <c r="AY1" s="23"/>
+      <c r="AZ1" s="23"/>
+      <c r="BA1" s="23"/>
+      <c r="BB1" s="23"/>
       <c r="BC1" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>39</v>
@@ -946,36 +946,36 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:55" x14ac:dyDescent="0.25">
       <c r="BC3" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:55" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="22" t="s">
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="24"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="22"/>
       <c r="BC4" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>41</v>
@@ -983,51 +983,51 @@
       <c r="D5" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="15">
-        <v>0</v>
-      </c>
-      <c r="F5" s="16">
-        <v>0</v>
-      </c>
-      <c r="G5" s="16">
-        <v>0</v>
-      </c>
-      <c r="H5" s="16">
-        <v>0</v>
-      </c>
-      <c r="I5" s="16">
-        <v>0</v>
-      </c>
-      <c r="J5" s="16">
-        <v>0</v>
-      </c>
-      <c r="K5" s="16">
-        <v>0</v>
-      </c>
-      <c r="L5" s="16">
-        <v>1</v>
-      </c>
-      <c r="M5" s="17" t="s">
+      <c r="E5" s="13">
+        <v>0</v>
+      </c>
+      <c r="F5" s="14">
+        <v>0</v>
+      </c>
+      <c r="G5" s="14">
+        <v>0</v>
+      </c>
+      <c r="H5" s="14">
+        <v>0</v>
+      </c>
+      <c r="I5" s="14">
+        <v>0</v>
+      </c>
+      <c r="J5" s="14">
+        <v>0</v>
+      </c>
+      <c r="K5" s="14">
+        <v>0</v>
+      </c>
+      <c r="L5" s="14">
+        <v>1</v>
+      </c>
+      <c r="M5" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="N5" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
-      <c r="S5" s="10"/>
-      <c r="T5" s="10"/>
-      <c r="U5" s="10"/>
+      <c r="N5" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
+      <c r="U5" s="23"/>
       <c r="BC5" s="9" t="str">
         <f t="shared" si="0"/>
         <v>End Command</v>
       </c>
     </row>
-    <row r="6" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>42</v>
@@ -1035,51 +1035,51 @@
       <c r="D6" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="13">
-        <v>0</v>
-      </c>
-      <c r="F6" s="14">
-        <v>0</v>
-      </c>
-      <c r="G6" s="14">
-        <v>0</v>
-      </c>
-      <c r="H6" s="14">
-        <v>0</v>
-      </c>
-      <c r="I6" s="14">
-        <v>0</v>
-      </c>
-      <c r="J6" s="14">
-        <v>0</v>
-      </c>
-      <c r="K6" s="14">
-        <v>1</v>
-      </c>
-      <c r="L6" s="14">
-        <v>0</v>
-      </c>
-      <c r="M6" s="18" t="s">
+      <c r="E6" s="11">
+        <v>0</v>
+      </c>
+      <c r="F6" s="12">
+        <v>0</v>
+      </c>
+      <c r="G6" s="12">
+        <v>0</v>
+      </c>
+      <c r="H6" s="12">
+        <v>0</v>
+      </c>
+      <c r="I6" s="12">
+        <v>0</v>
+      </c>
+      <c r="J6" s="12">
+        <v>0</v>
+      </c>
+      <c r="K6" s="12">
+        <v>1</v>
+      </c>
+      <c r="L6" s="12">
+        <v>0</v>
+      </c>
+      <c r="M6" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="N6" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="10"/>
-      <c r="T6" s="10"/>
-      <c r="U6" s="10"/>
+      <c r="N6" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="23"/>
+      <c r="T6" s="23"/>
+      <c r="U6" s="23"/>
       <c r="BC6" s="9" t="str">
         <f t="shared" si="0"/>
         <v>End Command</v>
       </c>
     </row>
-    <row r="7" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>43</v>
@@ -1087,51 +1087,51 @@
       <c r="D7" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="13">
-        <v>0</v>
-      </c>
-      <c r="F7" s="14">
-        <v>0</v>
-      </c>
-      <c r="G7" s="14">
-        <v>0</v>
-      </c>
-      <c r="H7" s="14">
-        <v>0</v>
-      </c>
-      <c r="I7" s="14">
-        <v>0</v>
-      </c>
-      <c r="J7" s="14">
-        <v>0</v>
-      </c>
-      <c r="K7" s="14">
-        <v>1</v>
-      </c>
-      <c r="L7" s="14">
-        <v>1</v>
-      </c>
-      <c r="M7" s="18" t="s">
+      <c r="E7" s="11">
+        <v>0</v>
+      </c>
+      <c r="F7" s="12">
+        <v>0</v>
+      </c>
+      <c r="G7" s="12">
+        <v>0</v>
+      </c>
+      <c r="H7" s="12">
+        <v>0</v>
+      </c>
+      <c r="I7" s="12">
+        <v>0</v>
+      </c>
+      <c r="J7" s="12">
+        <v>0</v>
+      </c>
+      <c r="K7" s="12">
+        <v>1</v>
+      </c>
+      <c r="L7" s="12">
+        <v>1</v>
+      </c>
+      <c r="M7" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="N7" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="10"/>
-      <c r="S7" s="10"/>
-      <c r="T7" s="10"/>
-      <c r="U7" s="10"/>
+      <c r="N7" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="23"/>
+      <c r="U7" s="23"/>
       <c r="BC7" s="9" t="str">
         <f t="shared" si="0"/>
         <v>End Command</v>
       </c>
     </row>
-    <row r="8" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>44</v>
@@ -1139,78 +1139,78 @@
       <c r="D8" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="19">
-        <v>0</v>
-      </c>
-      <c r="F8" s="20">
-        <v>0</v>
-      </c>
-      <c r="G8" s="20">
-        <v>0</v>
-      </c>
-      <c r="H8" s="20">
-        <v>0</v>
-      </c>
-      <c r="I8" s="20">
-        <v>0</v>
-      </c>
-      <c r="J8" s="20">
-        <v>1</v>
-      </c>
-      <c r="K8" s="20">
-        <v>0</v>
-      </c>
-      <c r="L8" s="20">
-        <v>0</v>
-      </c>
-      <c r="M8" s="21" t="s">
+      <c r="E8" s="17">
+        <v>0</v>
+      </c>
+      <c r="F8" s="18">
+        <v>0</v>
+      </c>
+      <c r="G8" s="18">
+        <v>0</v>
+      </c>
+      <c r="H8" s="18">
+        <v>0</v>
+      </c>
+      <c r="I8" s="18">
+        <v>0</v>
+      </c>
+      <c r="J8" s="18">
+        <v>1</v>
+      </c>
+      <c r="K8" s="18">
+        <v>0</v>
+      </c>
+      <c r="L8" s="18">
+        <v>0</v>
+      </c>
+      <c r="M8" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="N8" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
-      <c r="S8" s="10"/>
-      <c r="T8" s="10"/>
-      <c r="U8" s="10"/>
+      <c r="N8" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="23"/>
+      <c r="S8" s="23"/>
+      <c r="T8" s="23"/>
+      <c r="U8" s="23"/>
       <c r="BC8" s="9" t="str">
         <f t="shared" si="0"/>
         <v>End Command</v>
       </c>
     </row>
-    <row r="9" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:55" x14ac:dyDescent="0.25">
       <c r="BC9" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:55" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="22" t="s">
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="24"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="22"/>
       <c r="BC10" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>49</v>
@@ -1218,31 +1218,31 @@
       <c r="D11" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="15">
-        <v>0</v>
-      </c>
-      <c r="F11" s="16">
-        <v>0</v>
-      </c>
-      <c r="G11" s="16">
-        <v>0</v>
-      </c>
-      <c r="H11" s="16">
-        <v>1</v>
-      </c>
-      <c r="I11" s="16">
-        <v>0</v>
-      </c>
-      <c r="J11" s="16">
-        <v>0</v>
-      </c>
-      <c r="K11" s="16">
-        <v>0</v>
-      </c>
-      <c r="L11" s="16">
-        <v>1</v>
-      </c>
-      <c r="M11" s="17" t="s">
+      <c r="E11" s="13">
+        <v>0</v>
+      </c>
+      <c r="F11" s="14">
+        <v>0</v>
+      </c>
+      <c r="G11" s="14">
+        <v>0</v>
+      </c>
+      <c r="H11" s="14">
+        <v>1</v>
+      </c>
+      <c r="I11" s="14">
+        <v>0</v>
+      </c>
+      <c r="J11" s="14">
+        <v>0</v>
+      </c>
+      <c r="K11" s="14">
+        <v>0</v>
+      </c>
+      <c r="L11" s="14">
+        <v>1</v>
+      </c>
+      <c r="M11" s="15" t="s">
         <v>56</v>
       </c>
       <c r="BC11" s="9" t="str">
@@ -1250,9 +1250,9 @@
         <v>End Command</v>
       </c>
     </row>
-    <row r="12" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>50</v>
@@ -1260,31 +1260,31 @@
       <c r="D12" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="13">
-        <v>0</v>
-      </c>
-      <c r="F12" s="14">
-        <v>0</v>
-      </c>
-      <c r="G12" s="14">
-        <v>0</v>
-      </c>
-      <c r="H12" s="14">
-        <v>1</v>
-      </c>
-      <c r="I12" s="14">
-        <v>0</v>
-      </c>
-      <c r="J12" s="14">
-        <v>0</v>
-      </c>
-      <c r="K12" s="14">
-        <v>1</v>
-      </c>
-      <c r="L12" s="14">
-        <v>0</v>
-      </c>
-      <c r="M12" s="18" t="s">
+      <c r="E12" s="11">
+        <v>0</v>
+      </c>
+      <c r="F12" s="12">
+        <v>0</v>
+      </c>
+      <c r="G12" s="12">
+        <v>0</v>
+      </c>
+      <c r="H12" s="12">
+        <v>1</v>
+      </c>
+      <c r="I12" s="12">
+        <v>0</v>
+      </c>
+      <c r="J12" s="12">
+        <v>0</v>
+      </c>
+      <c r="K12" s="12">
+        <v>1</v>
+      </c>
+      <c r="L12" s="12">
+        <v>0</v>
+      </c>
+      <c r="M12" s="16" t="s">
         <v>57</v>
       </c>
       <c r="BC12" s="9" t="str">
@@ -1292,9 +1292,9 @@
         <v>End Command</v>
       </c>
     </row>
-    <row r="13" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>51</v>
@@ -1302,31 +1302,31 @@
       <c r="D13" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="19">
-        <v>0</v>
-      </c>
-      <c r="F13" s="20">
-        <v>0</v>
-      </c>
-      <c r="G13" s="20">
-        <v>0</v>
-      </c>
-      <c r="H13" s="20">
-        <v>1</v>
-      </c>
-      <c r="I13" s="20">
-        <v>0</v>
-      </c>
-      <c r="J13" s="20">
-        <v>0</v>
-      </c>
-      <c r="K13" s="20">
-        <v>1</v>
-      </c>
-      <c r="L13" s="20">
-        <v>1</v>
-      </c>
-      <c r="M13" s="21" t="s">
+      <c r="E13" s="17">
+        <v>0</v>
+      </c>
+      <c r="F13" s="18">
+        <v>0</v>
+      </c>
+      <c r="G13" s="18">
+        <v>0</v>
+      </c>
+      <c r="H13" s="18">
+        <v>1</v>
+      </c>
+      <c r="I13" s="18">
+        <v>0</v>
+      </c>
+      <c r="J13" s="18">
+        <v>0</v>
+      </c>
+      <c r="K13" s="18">
+        <v>1</v>
+      </c>
+      <c r="L13" s="18">
+        <v>1</v>
+      </c>
+      <c r="M13" s="19" t="s">
         <v>58</v>
       </c>
       <c r="BC13" s="9" t="str">
@@ -1334,91 +1334,91 @@
         <v>End Command</v>
       </c>
     </row>
-    <row r="14" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:55" x14ac:dyDescent="0.25">
       <c r="BC14" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="23"/>
-      <c r="M15" s="23"/>
-      <c r="N15" s="23"/>
-      <c r="O15" s="23"/>
-      <c r="P15" s="23"/>
-      <c r="Q15" s="23"/>
-      <c r="R15" s="23"/>
-      <c r="S15" s="23"/>
-      <c r="T15" s="23"/>
-      <c r="U15" s="23"/>
-      <c r="V15" s="24"/>
+      <c r="E15" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="21"/>
+      <c r="O15" s="21"/>
+      <c r="P15" s="21"/>
+      <c r="Q15" s="21"/>
+      <c r="R15" s="21"/>
+      <c r="S15" s="21"/>
+      <c r="T15" s="21"/>
+      <c r="U15" s="21"/>
+      <c r="V15" s="22"/>
       <c r="BC15" s="9" t="str">
         <f t="shared" si="0"/>
         <v>End Command</v>
       </c>
     </row>
-    <row r="16" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:55" x14ac:dyDescent="0.25">
       <c r="BC16" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="17" spans="7:55" x14ac:dyDescent="0.3">
+    <row r="17" spans="7:55" x14ac:dyDescent="0.25">
       <c r="BC17" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="18" spans="7:55" x14ac:dyDescent="0.3">
+    <row r="18" spans="7:55" x14ac:dyDescent="0.25">
       <c r="BC18" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="19" spans="7:55" x14ac:dyDescent="0.3">
+    <row r="19" spans="7:55" x14ac:dyDescent="0.25">
       <c r="BC19" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="20" spans="7:55" x14ac:dyDescent="0.3">
+    <row r="20" spans="7:55" x14ac:dyDescent="0.25">
       <c r="BC20" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="21" spans="7:55" x14ac:dyDescent="0.3">
-      <c r="G21" s="14">
-        <v>0</v>
-      </c>
-      <c r="H21" s="14">
-        <v>0</v>
-      </c>
-      <c r="I21" s="14">
-        <v>0</v>
-      </c>
-      <c r="J21" s="14">
-        <v>0</v>
-      </c>
-      <c r="M21" s="12" t="s">
+    <row r="21" spans="7:55" x14ac:dyDescent="0.25">
+      <c r="G21" s="12">
+        <v>0</v>
+      </c>
+      <c r="H21" s="12">
+        <v>0</v>
+      </c>
+      <c r="I21" s="12">
+        <v>0</v>
+      </c>
+      <c r="J21" s="12">
+        <v>0</v>
+      </c>
+      <c r="M21" s="10" t="s">
         <v>63</v>
       </c>
       <c r="BC21" s="9" t="str">
@@ -1426,20 +1426,20 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="7:55" x14ac:dyDescent="0.3">
-      <c r="G22" s="14">
-        <v>0</v>
-      </c>
-      <c r="H22" s="14">
-        <v>0</v>
-      </c>
-      <c r="I22" s="14">
-        <v>0</v>
-      </c>
-      <c r="J22" s="14">
-        <v>1</v>
-      </c>
-      <c r="M22" s="12" t="s">
+    <row r="22" spans="7:55" x14ac:dyDescent="0.25">
+      <c r="G22" s="12">
+        <v>0</v>
+      </c>
+      <c r="H22" s="12">
+        <v>0</v>
+      </c>
+      <c r="I22" s="12">
+        <v>0</v>
+      </c>
+      <c r="J22" s="12">
+        <v>1</v>
+      </c>
+      <c r="M22" s="10" t="s">
         <v>52</v>
       </c>
       <c r="BC22" s="9" t="str">
@@ -1447,20 +1447,20 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="7:55" x14ac:dyDescent="0.3">
-      <c r="G23" s="14">
-        <v>0</v>
-      </c>
-      <c r="H23" s="14">
-        <v>0</v>
-      </c>
-      <c r="I23" s="14">
-        <v>1</v>
-      </c>
-      <c r="J23" s="14">
-        <v>0</v>
-      </c>
-      <c r="M23" s="12" t="s">
+    <row r="23" spans="7:55" x14ac:dyDescent="0.25">
+      <c r="G23" s="12">
+        <v>0</v>
+      </c>
+      <c r="H23" s="12">
+        <v>0</v>
+      </c>
+      <c r="I23" s="12">
+        <v>1</v>
+      </c>
+      <c r="J23" s="12">
+        <v>0</v>
+      </c>
+      <c r="M23" s="10" t="s">
         <v>53</v>
       </c>
       <c r="BC23" s="9" t="str">
@@ -1468,20 +1468,20 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="7:55" x14ac:dyDescent="0.3">
-      <c r="G24" s="14">
-        <v>0</v>
-      </c>
-      <c r="H24" s="14">
-        <v>0</v>
-      </c>
-      <c r="I24" s="14">
-        <v>1</v>
-      </c>
-      <c r="J24" s="14">
-        <v>1</v>
-      </c>
-      <c r="M24" s="12" t="s">
+    <row r="24" spans="7:55" x14ac:dyDescent="0.25">
+      <c r="G24" s="12">
+        <v>0</v>
+      </c>
+      <c r="H24" s="12">
+        <v>0</v>
+      </c>
+      <c r="I24" s="12">
+        <v>1</v>
+      </c>
+      <c r="J24" s="12">
+        <v>1</v>
+      </c>
+      <c r="M24" s="10" t="s">
         <v>54</v>
       </c>
       <c r="BC24" s="9" t="str">
@@ -1489,20 +1489,20 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="7:55" x14ac:dyDescent="0.3">
-      <c r="G25" s="14">
-        <v>0</v>
-      </c>
-      <c r="H25" s="14">
-        <v>1</v>
-      </c>
-      <c r="I25" s="14">
-        <v>0</v>
-      </c>
-      <c r="J25" s="14">
-        <v>0</v>
-      </c>
-      <c r="M25" s="12" t="s">
+    <row r="25" spans="7:55" x14ac:dyDescent="0.25">
+      <c r="G25" s="12">
+        <v>0</v>
+      </c>
+      <c r="H25" s="12">
+        <v>1</v>
+      </c>
+      <c r="I25" s="12">
+        <v>0</v>
+      </c>
+      <c r="J25" s="12">
+        <v>0</v>
+      </c>
+      <c r="M25" s="10" t="s">
         <v>55</v>
       </c>
       <c r="BC25" s="9" t="str">
@@ -1510,20 +1510,20 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="7:55" x14ac:dyDescent="0.3">
-      <c r="G26" s="14">
-        <v>0</v>
-      </c>
-      <c r="H26" s="14">
-        <v>1</v>
-      </c>
-      <c r="I26" s="14">
-        <v>0</v>
-      </c>
-      <c r="J26" s="14">
-        <v>1</v>
-      </c>
-      <c r="M26" s="12" t="s">
+    <row r="26" spans="7:55" x14ac:dyDescent="0.25">
+      <c r="G26" s="12">
+        <v>0</v>
+      </c>
+      <c r="H26" s="12">
+        <v>1</v>
+      </c>
+      <c r="I26" s="12">
+        <v>0</v>
+      </c>
+      <c r="J26" s="12">
+        <v>1</v>
+      </c>
+      <c r="M26" s="10" t="s">
         <v>59</v>
       </c>
       <c r="BC26" s="9" t="str">
@@ -1531,20 +1531,20 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="7:55" x14ac:dyDescent="0.3">
-      <c r="G27" s="14">
-        <v>0</v>
-      </c>
-      <c r="H27" s="14">
-        <v>1</v>
-      </c>
-      <c r="I27" s="14">
-        <v>1</v>
-      </c>
-      <c r="J27" s="14">
-        <v>0</v>
-      </c>
-      <c r="M27" s="12" t="s">
+    <row r="27" spans="7:55" x14ac:dyDescent="0.25">
+      <c r="G27" s="12">
+        <v>0</v>
+      </c>
+      <c r="H27" s="12">
+        <v>1</v>
+      </c>
+      <c r="I27" s="12">
+        <v>1</v>
+      </c>
+      <c r="J27" s="12">
+        <v>0</v>
+      </c>
+      <c r="M27" s="10" t="s">
         <v>60</v>
       </c>
       <c r="BC27" s="9" t="str">
@@ -1552,20 +1552,20 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="7:55" x14ac:dyDescent="0.3">
-      <c r="G28" s="14">
-        <v>0</v>
-      </c>
-      <c r="H28" s="14">
-        <v>1</v>
-      </c>
-      <c r="I28" s="14">
-        <v>1</v>
-      </c>
-      <c r="J28" s="14">
-        <v>1</v>
-      </c>
-      <c r="M28" s="12" t="s">
+    <row r="28" spans="7:55" x14ac:dyDescent="0.25">
+      <c r="G28" s="12">
+        <v>0</v>
+      </c>
+      <c r="H28" s="12">
+        <v>1</v>
+      </c>
+      <c r="I28" s="12">
+        <v>1</v>
+      </c>
+      <c r="J28" s="12">
+        <v>1</v>
+      </c>
+      <c r="M28" s="10" t="s">
         <v>61</v>
       </c>
       <c r="BC28" s="9" t="str">
@@ -1573,20 +1573,20 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="7:55" x14ac:dyDescent="0.3">
-      <c r="G29" s="14">
-        <v>1</v>
-      </c>
-      <c r="H29" s="14">
-        <v>0</v>
-      </c>
-      <c r="I29" s="14">
-        <v>0</v>
-      </c>
-      <c r="J29" s="14">
-        <v>0</v>
-      </c>
-      <c r="M29" s="12" t="s">
+    <row r="29" spans="7:55" x14ac:dyDescent="0.25">
+      <c r="G29" s="12">
+        <v>1</v>
+      </c>
+      <c r="H29" s="12">
+        <v>0</v>
+      </c>
+      <c r="I29" s="12">
+        <v>0</v>
+      </c>
+      <c r="J29" s="12">
+        <v>0</v>
+      </c>
+      <c r="M29" s="10" t="s">
         <v>62</v>
       </c>
       <c r="BC29" s="9" t="str">
@@ -1594,20 +1594,20 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="7:55" x14ac:dyDescent="0.3">
-      <c r="G30" s="14">
-        <v>1</v>
-      </c>
-      <c r="H30" s="14">
-        <v>0</v>
-      </c>
-      <c r="I30" s="14">
-        <v>0</v>
-      </c>
-      <c r="J30" s="14">
-        <v>1</v>
-      </c>
-      <c r="M30" s="12" t="s">
+    <row r="30" spans="7:55" x14ac:dyDescent="0.25">
+      <c r="G30" s="12">
+        <v>1</v>
+      </c>
+      <c r="H30" s="12">
+        <v>0</v>
+      </c>
+      <c r="I30" s="12">
+        <v>0</v>
+      </c>
+      <c r="J30" s="12">
+        <v>1</v>
+      </c>
+      <c r="M30" s="10" t="s">
         <v>64</v>
       </c>
       <c r="BC30" s="9" t="str">
@@ -1615,20 +1615,20 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="7:55" x14ac:dyDescent="0.3">
-      <c r="G31" s="14">
-        <v>1</v>
-      </c>
-      <c r="H31" s="14">
-        <v>0</v>
-      </c>
-      <c r="I31" s="14">
-        <v>1</v>
-      </c>
-      <c r="J31" s="14">
-        <v>0</v>
-      </c>
-      <c r="M31" s="12" t="s">
+    <row r="31" spans="7:55" x14ac:dyDescent="0.25">
+      <c r="G31" s="12">
+        <v>1</v>
+      </c>
+      <c r="H31" s="12">
+        <v>0</v>
+      </c>
+      <c r="I31" s="12">
+        <v>1</v>
+      </c>
+      <c r="J31" s="12">
+        <v>0</v>
+      </c>
+      <c r="M31" s="10" t="s">
         <v>65</v>
       </c>
       <c r="BC31" s="9" t="str">
@@ -1636,20 +1636,20 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="7:55" x14ac:dyDescent="0.3">
-      <c r="G32" s="14">
-        <v>1</v>
-      </c>
-      <c r="H32" s="14">
-        <v>0</v>
-      </c>
-      <c r="I32" s="14">
-        <v>1</v>
-      </c>
-      <c r="J32" s="14">
-        <v>1</v>
-      </c>
-      <c r="M32" s="12" t="s">
+    <row r="32" spans="7:55" x14ac:dyDescent="0.25">
+      <c r="G32" s="12">
+        <v>1</v>
+      </c>
+      <c r="H32" s="12">
+        <v>0</v>
+      </c>
+      <c r="I32" s="12">
+        <v>1</v>
+      </c>
+      <c r="J32" s="12">
+        <v>1</v>
+      </c>
+      <c r="M32" s="10" t="s">
         <v>66</v>
       </c>
       <c r="BC32" s="9" t="str">
@@ -1657,20 +1657,20 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="7:55" x14ac:dyDescent="0.3">
-      <c r="G33" s="14">
-        <v>1</v>
-      </c>
-      <c r="H33" s="14">
-        <v>1</v>
-      </c>
-      <c r="I33" s="14">
-        <v>0</v>
-      </c>
-      <c r="J33" s="14">
-        <v>0</v>
-      </c>
-      <c r="M33" s="12" t="s">
+    <row r="33" spans="7:55" x14ac:dyDescent="0.25">
+      <c r="G33" s="12">
+        <v>1</v>
+      </c>
+      <c r="H33" s="12">
+        <v>1</v>
+      </c>
+      <c r="I33" s="12">
+        <v>0</v>
+      </c>
+      <c r="J33" s="12">
+        <v>0</v>
+      </c>
+      <c r="M33" s="10" t="s">
         <v>67</v>
       </c>
       <c r="BC33" s="9" t="str">
@@ -1678,20 +1678,20 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="7:55" x14ac:dyDescent="0.3">
-      <c r="G34" s="14">
-        <v>1</v>
-      </c>
-      <c r="H34" s="14">
-        <v>1</v>
-      </c>
-      <c r="I34" s="14">
-        <v>0</v>
-      </c>
-      <c r="J34" s="14">
-        <v>1</v>
-      </c>
-      <c r="M34" s="12" t="s">
+    <row r="34" spans="7:55" x14ac:dyDescent="0.25">
+      <c r="G34" s="12">
+        <v>1</v>
+      </c>
+      <c r="H34" s="12">
+        <v>1</v>
+      </c>
+      <c r="I34" s="12">
+        <v>0</v>
+      </c>
+      <c r="J34" s="12">
+        <v>1</v>
+      </c>
+      <c r="M34" s="10" t="s">
         <v>68</v>
       </c>
       <c r="BC34" s="9" t="str">
@@ -1699,20 +1699,20 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="7:55" x14ac:dyDescent="0.3">
-      <c r="G35" s="14">
-        <v>1</v>
-      </c>
-      <c r="H35" s="14">
-        <v>1</v>
-      </c>
-      <c r="I35" s="14">
-        <v>1</v>
-      </c>
-      <c r="J35" s="14">
-        <v>0</v>
-      </c>
-      <c r="M35" s="12" t="s">
+    <row r="35" spans="7:55" x14ac:dyDescent="0.25">
+      <c r="G35" s="12">
+        <v>1</v>
+      </c>
+      <c r="H35" s="12">
+        <v>1</v>
+      </c>
+      <c r="I35" s="12">
+        <v>1</v>
+      </c>
+      <c r="J35" s="12">
+        <v>0</v>
+      </c>
+      <c r="M35" s="10" t="s">
         <v>69</v>
       </c>
       <c r="BC35" s="9" t="str">
@@ -1720,20 +1720,20 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="7:55" x14ac:dyDescent="0.3">
-      <c r="G36" s="14">
-        <v>1</v>
-      </c>
-      <c r="H36" s="14">
-        <v>1</v>
-      </c>
-      <c r="I36" s="14">
-        <v>1</v>
-      </c>
-      <c r="J36" s="14">
-        <v>1</v>
-      </c>
-      <c r="M36" s="12" t="s">
+    <row r="36" spans="7:55" x14ac:dyDescent="0.25">
+      <c r="G36" s="12">
+        <v>1</v>
+      </c>
+      <c r="H36" s="12">
+        <v>1</v>
+      </c>
+      <c r="I36" s="12">
+        <v>1</v>
+      </c>
+      <c r="J36" s="12">
+        <v>1</v>
+      </c>
+      <c r="M36" s="10" t="s">
         <v>70</v>
       </c>
       <c r="BC36" s="9" t="str">
@@ -1741,91 +1741,91 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="7:55" x14ac:dyDescent="0.3">
+    <row r="37" spans="7:55" x14ac:dyDescent="0.25">
       <c r="BC37" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="38" spans="7:55" x14ac:dyDescent="0.3">
+    <row r="38" spans="7:55" x14ac:dyDescent="0.25">
       <c r="BC38" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="39" spans="7:55" x14ac:dyDescent="0.3">
+    <row r="39" spans="7:55" x14ac:dyDescent="0.25">
       <c r="BC39" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="40" spans="7:55" x14ac:dyDescent="0.3">
+    <row r="40" spans="7:55" x14ac:dyDescent="0.25">
       <c r="BC40" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="41" spans="7:55" x14ac:dyDescent="0.3">
+    <row r="41" spans="7:55" x14ac:dyDescent="0.25">
       <c r="BC41" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="42" spans="7:55" x14ac:dyDescent="0.3">
+    <row r="42" spans="7:55" x14ac:dyDescent="0.25">
       <c r="BC42" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="43" spans="7:55" x14ac:dyDescent="0.3">
+    <row r="43" spans="7:55" x14ac:dyDescent="0.25">
       <c r="BC43" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="44" spans="7:55" x14ac:dyDescent="0.3">
+    <row r="44" spans="7:55" x14ac:dyDescent="0.25">
       <c r="BC44" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="45" spans="7:55" x14ac:dyDescent="0.3">
+    <row r="45" spans="7:55" x14ac:dyDescent="0.25">
       <c r="BC45" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="46" spans="7:55" x14ac:dyDescent="0.3">
+    <row r="46" spans="7:55" x14ac:dyDescent="0.25">
       <c r="BC46" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="47" spans="7:55" x14ac:dyDescent="0.3">
+    <row r="47" spans="7:55" x14ac:dyDescent="0.25">
       <c r="BC47" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="48" spans="7:55" x14ac:dyDescent="0.3">
+    <row r="48" spans="7:55" x14ac:dyDescent="0.25">
       <c r="BC48" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="49" spans="55:55" x14ac:dyDescent="0.3">
+    <row r="49" spans="55:55" x14ac:dyDescent="0.25">
       <c r="BC49" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="50" spans="55:55" x14ac:dyDescent="0.3">
+    <row r="50" spans="55:55" x14ac:dyDescent="0.25">
       <c r="BC50" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="51" spans="55:55" x14ac:dyDescent="0.3">
+    <row r="51" spans="55:55" x14ac:dyDescent="0.25">
       <c r="BC51" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1862,17 +1862,17 @@
       <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="9.109375" style="1"/>
-    <col min="10" max="10" width="10.5546875" style="1" customWidth="1"/>
-    <col min="11" max="13" width="10.5546875" style="7" customWidth="1"/>
-    <col min="14" max="14" width="9.109375" style="2"/>
-    <col min="15" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="10.5703125" style="1" customWidth="1"/>
+    <col min="11" max="13" width="10.5703125" style="7" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="2"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1910,7 +1910,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -1944,7 +1944,7 @@
       <c r="AC2" s="8"/>
       <c r="AD2" s="8"/>
     </row>
-    <row r="3" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1962,7 +1962,7 @@
       </c>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -1992,7 +1992,7 @@
       </c>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -2124,7 +2124,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -2190,7 +2190,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
@@ -2256,7 +2256,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -2276,7 +2276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -2296,7 +2296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -2316,7 +2316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -2336,7 +2336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -2356,7 +2356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -2376,7 +2376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -2396,7 +2396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -2408,7 +2408,7 @@
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -2420,7 +2420,7 @@
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -2432,7 +2432,7 @@
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
     </row>
-    <row r="24" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>3</v>
       </c>
@@ -2450,7 +2450,7 @@
       </c>
       <c r="N24" s="2"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>15</v>
       </c>
@@ -2482,7 +2482,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>16</v>
       </c>
@@ -2514,7 +2514,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>17</v>
       </c>
@@ -2546,7 +2546,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>18</v>
       </c>
@@ -2578,7 +2578,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>19</v>
       </c>
@@ -2610,7 +2610,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="G30" s="4">
         <v>0</v>
@@ -2625,7 +2625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="G31" s="4">
         <v>0</v>
@@ -2640,7 +2640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="G32" s="4">
         <v>0</v>
@@ -2655,7 +2655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="G33" s="4">
         <v>1</v>
@@ -2670,7 +2670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="G34" s="4">
         <v>1</v>
@@ -2685,7 +2685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="G35" s="4">
         <v>1</v>
@@ -2700,7 +2700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="G36" s="4">
         <v>1</v>
@@ -2715,7 +2715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="G37" s="4">
         <v>1</v>
@@ -2730,7 +2730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="G38" s="4">
         <v>1</v>
@@ -2745,7 +2745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="G39" s="4">
         <v>1</v>
@@ -2760,7 +2760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="G40" s="4">
         <v>1</v>

</xml_diff>

<commit_message>
updating packet protocol, prepping finalCompetition documentation
</commit_message>
<xml_diff>
--- a/Command_Data Planner.xlsx
+++ b/Command_Data Planner.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Materia\2022 Spring\Courses\ECPE-155 Autonomous Robotics\Labs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emily\bishop_ecpe155_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE56F7D-2707-4F73-8C50-9E78021543FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C6311D-2249-4D1F-9FDA-2E17B0CE8172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{41C8675F-361B-4635-AFD0-4B5E8933C9D2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{41C8675F-361B-4635-AFD0-4B5E8933C9D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Packet Protocol" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="94">
   <si>
     <t xml:space="preserve">command </t>
   </si>
@@ -263,13 +263,61 @@
     <t>Tiva</t>
   </si>
   <si>
-    <t>2 Bytes of Data (max = 65535)</t>
-  </si>
-  <si>
     <t>Send IR Value</t>
   </si>
   <si>
     <t>Distance (cm)</t>
+  </si>
+  <si>
+    <t>0x96</t>
+  </si>
+  <si>
+    <t>obstacle avoidance</t>
+  </si>
+  <si>
+    <t>isStopped</t>
+  </si>
+  <si>
+    <t>OBSTACLE DETECTION</t>
+  </si>
+  <si>
+    <t>front IRs detected</t>
+  </si>
+  <si>
+    <t>isFrontIR</t>
+  </si>
+  <si>
+    <t>isBlueCircle</t>
+  </si>
+  <si>
+    <t>isGoal</t>
+  </si>
+  <si>
+    <t>2 Bytes of Data (max int = 65535)</t>
+  </si>
+  <si>
+    <t>DISTANCE</t>
+  </si>
+  <si>
+    <t>quad enc avg values</t>
+  </si>
+  <si>
+    <t>avgQENum 2 Bytes of Data (max int = 65535)</t>
+  </si>
+  <si>
+    <t>turn at n*45 angle (every stop)</t>
+  </si>
+  <si>
+    <t>send n num of angles</t>
+  </si>
+  <si>
+    <t>seesWaypoint</t>
+  </si>
+  <si>
+    <t>noWaypoint</t>
+  </si>
+  <si>
+    <t>numOfAngles</t>
   </si>
 </sst>
 </file>
@@ -335,7 +383,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -466,11 +514,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -498,19 +557,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -526,6 +586,39 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -842,1012 +935,1514 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85CA0D59-C129-4927-BBCA-0FC73B637AB1}">
-  <dimension ref="A1:BC51"/>
+  <dimension ref="A1:BG58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8:U8"/>
+      <selection activeCell="U24" sqref="U24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="9"/>
-    <col min="2" max="2" width="15.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="9"/>
-    <col min="4" max="4" width="14.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="12" width="2.7109375" style="12" customWidth="1"/>
-    <col min="13" max="13" width="6.7109375" style="10" customWidth="1"/>
-    <col min="14" max="21" width="2.7109375" style="9" customWidth="1"/>
-    <col min="22" max="22" width="6.7109375" style="1" customWidth="1"/>
-    <col min="23" max="54" width="2.7109375" style="9" customWidth="1"/>
-    <col min="55" max="55" width="13.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="56" max="16384" width="8.85546875" style="9"/>
+    <col min="1" max="1" width="8.88671875" style="9"/>
+    <col min="2" max="2" width="25.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="9"/>
+    <col min="4" max="4" width="14.5546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="12" width="2.6640625" style="16" customWidth="1"/>
+    <col min="13" max="13" width="6.6640625" style="16" customWidth="1"/>
+    <col min="14" max="21" width="2.6640625" style="15" customWidth="1"/>
+    <col min="22" max="22" width="6.6640625" style="15" customWidth="1"/>
+    <col min="23" max="30" width="2.6640625" style="15" customWidth="1"/>
+    <col min="31" max="31" width="6.6640625" style="15" customWidth="1"/>
+    <col min="32" max="39" width="2.6640625" style="15" customWidth="1"/>
+    <col min="40" max="40" width="6.6640625" style="15" customWidth="1"/>
+    <col min="41" max="48" width="2.6640625" style="15" customWidth="1"/>
+    <col min="49" max="49" width="6.6640625" style="15" customWidth="1"/>
+    <col min="50" max="57" width="2.6640625" style="15" customWidth="1"/>
+    <col min="58" max="58" width="6.6640625" style="15" customWidth="1"/>
+    <col min="59" max="59" width="13.88671875" style="15" bestFit="1" customWidth="1"/>
+    <col min="60" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:59" x14ac:dyDescent="0.3">
       <c r="C1" s="9" t="s">
         <v>46</v>
       </c>
       <c r="D1" s="1">
         <v>1</v>
       </c>
-      <c r="E1" s="24">
+      <c r="E1" s="21">
         <v>2</v>
       </c>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="N1" s="23">
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="20">
         <v>3</v>
       </c>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="W1" s="23">
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="20">
         <v>4</v>
       </c>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="23"/>
-      <c r="AB1" s="23"/>
-      <c r="AC1" s="23"/>
-      <c r="AD1" s="23"/>
-      <c r="AE1" s="23">
+      <c r="X1" s="20"/>
+      <c r="Y1" s="20"/>
+      <c r="Z1" s="20"/>
+      <c r="AA1" s="20"/>
+      <c r="AB1" s="20"/>
+      <c r="AC1" s="20"/>
+      <c r="AD1" s="20"/>
+      <c r="AF1" s="20">
         <v>5</v>
       </c>
-      <c r="AF1" s="23"/>
-      <c r="AG1" s="23"/>
-      <c r="AH1" s="23"/>
-      <c r="AI1" s="23"/>
-      <c r="AJ1" s="23"/>
-      <c r="AK1" s="23"/>
-      <c r="AL1" s="23"/>
-      <c r="AM1" s="23">
+      <c r="AG1" s="20"/>
+      <c r="AH1" s="20"/>
+      <c r="AI1" s="20"/>
+      <c r="AJ1" s="20"/>
+      <c r="AK1" s="20"/>
+      <c r="AL1" s="20"/>
+      <c r="AM1" s="20"/>
+      <c r="AO1" s="20">
         <v>6</v>
       </c>
-      <c r="AN1" s="23"/>
-      <c r="AO1" s="23"/>
-      <c r="AP1" s="23"/>
-      <c r="AQ1" s="23"/>
-      <c r="AR1" s="23"/>
-      <c r="AS1" s="23"/>
-      <c r="AT1" s="23"/>
-      <c r="AU1" s="23">
+      <c r="AP1" s="20"/>
+      <c r="AQ1" s="20"/>
+      <c r="AR1" s="20"/>
+      <c r="AS1" s="20"/>
+      <c r="AT1" s="20"/>
+      <c r="AU1" s="20"/>
+      <c r="AV1" s="20"/>
+      <c r="AX1" s="20">
         <v>7</v>
       </c>
-      <c r="AV1" s="23"/>
-      <c r="AW1" s="23"/>
-      <c r="AX1" s="23"/>
-      <c r="AY1" s="23"/>
-      <c r="AZ1" s="23"/>
-      <c r="BA1" s="23"/>
-      <c r="BB1" s="23"/>
-      <c r="BC1" s="1">
+      <c r="AY1" s="20"/>
+      <c r="AZ1" s="20"/>
+      <c r="BA1" s="20"/>
+      <c r="BB1" s="20"/>
+      <c r="BC1" s="20"/>
+      <c r="BD1" s="20"/>
+      <c r="BE1" s="20"/>
+      <c r="BG1" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>72</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="BC2" s="9" t="str">
-        <f t="shared" ref="BC2:BC51" si="0">IF($D2 = "Start Command", "End Command", "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="3" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="BC3" s="9" t="str">
+      <c r="D2" s="9"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="9"/>
+      <c r="Z2" s="9"/>
+      <c r="AA2" s="9"/>
+      <c r="AB2" s="9"/>
+      <c r="AC2" s="9"/>
+      <c r="AD2" s="9"/>
+      <c r="AF2" s="9"/>
+      <c r="AG2" s="9"/>
+      <c r="AH2" s="9"/>
+      <c r="AI2" s="9"/>
+      <c r="AJ2" s="9"/>
+      <c r="AK2" s="9"/>
+      <c r="AL2" s="9"/>
+      <c r="AM2" s="9"/>
+      <c r="AO2" s="9"/>
+      <c r="AP2" s="9"/>
+      <c r="AQ2" s="9"/>
+      <c r="AR2" s="9"/>
+      <c r="AS2" s="9"/>
+      <c r="AT2" s="9"/>
+      <c r="AU2" s="9"/>
+      <c r="AV2" s="9"/>
+      <c r="AX2" s="9"/>
+      <c r="AY2" s="9"/>
+      <c r="AZ2" s="9"/>
+      <c r="BA2" s="9"/>
+      <c r="BB2" s="9"/>
+      <c r="BC2" s="9"/>
+      <c r="BD2" s="9"/>
+      <c r="BE2" s="9"/>
+      <c r="BG2" s="9" t="str">
+        <f t="shared" ref="BG2:BG20" si="0">IF($D2 = "Start Command", "End Command", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="BG3" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B4" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="20" t="s">
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="22"/>
-      <c r="BC4" s="9" t="str">
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="19"/>
+      <c r="BG4" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>73</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="13">
-        <v>0</v>
-      </c>
-      <c r="F5" s="14">
-        <v>0</v>
-      </c>
-      <c r="G5" s="14">
-        <v>0</v>
-      </c>
-      <c r="H5" s="14">
-        <v>0</v>
-      </c>
-      <c r="I5" s="14">
-        <v>0</v>
-      </c>
-      <c r="J5" s="14">
-        <v>0</v>
-      </c>
-      <c r="K5" s="14">
-        <v>0</v>
-      </c>
-      <c r="L5" s="14">
-        <v>1</v>
-      </c>
-      <c r="M5" s="15" t="s">
+      <c r="E5" s="26">
+        <v>0</v>
+      </c>
+      <c r="F5" s="23">
+        <v>0</v>
+      </c>
+      <c r="G5" s="23">
+        <v>0</v>
+      </c>
+      <c r="H5" s="23">
+        <v>0</v>
+      </c>
+      <c r="I5" s="23">
+        <v>0</v>
+      </c>
+      <c r="J5" s="23">
+        <v>0</v>
+      </c>
+      <c r="K5" s="23">
+        <v>0</v>
+      </c>
+      <c r="L5" s="23">
+        <v>1</v>
+      </c>
+      <c r="M5" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="N5" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="23"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="23"/>
-      <c r="U5" s="23"/>
-      <c r="BC5" s="9" t="str">
+      <c r="N5" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="20"/>
+      <c r="U5" s="20"/>
+      <c r="V5" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF5" s="20"/>
+      <c r="AG5" s="20"/>
+      <c r="AH5" s="20"/>
+      <c r="AI5" s="20"/>
+      <c r="AJ5" s="20"/>
+      <c r="AK5" s="20"/>
+      <c r="AL5" s="20"/>
+      <c r="AM5" s="20"/>
+      <c r="AO5" s="20"/>
+      <c r="AP5" s="20"/>
+      <c r="AQ5" s="20"/>
+      <c r="AR5" s="20"/>
+      <c r="AS5" s="20"/>
+      <c r="AT5" s="20"/>
+      <c r="AU5" s="20"/>
+      <c r="AV5" s="20"/>
+      <c r="AX5" s="20"/>
+      <c r="AY5" s="20"/>
+      <c r="AZ5" s="20"/>
+      <c r="BA5" s="20"/>
+      <c r="BB5" s="20"/>
+      <c r="BC5" s="20"/>
+      <c r="BD5" s="20"/>
+      <c r="BE5" s="20"/>
+      <c r="BG5" s="15" t="str">
         <f t="shared" si="0"/>
         <v>End Command</v>
       </c>
     </row>
-    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>73</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="11">
-        <v>0</v>
-      </c>
-      <c r="F6" s="12">
-        <v>0</v>
-      </c>
-      <c r="G6" s="12">
-        <v>0</v>
-      </c>
-      <c r="H6" s="12">
-        <v>0</v>
-      </c>
-      <c r="I6" s="12">
-        <v>0</v>
-      </c>
-      <c r="J6" s="12">
-        <v>0</v>
-      </c>
-      <c r="K6" s="12">
-        <v>1</v>
-      </c>
-      <c r="L6" s="12">
-        <v>0</v>
-      </c>
-      <c r="M6" s="16" t="s">
+      <c r="E6" s="27">
+        <v>0</v>
+      </c>
+      <c r="F6" s="16">
+        <v>0</v>
+      </c>
+      <c r="G6" s="16">
+        <v>0</v>
+      </c>
+      <c r="H6" s="16">
+        <v>0</v>
+      </c>
+      <c r="I6" s="16">
+        <v>0</v>
+      </c>
+      <c r="J6" s="16">
+        <v>0</v>
+      </c>
+      <c r="K6" s="16">
+        <v>1</v>
+      </c>
+      <c r="L6" s="16">
+        <v>0</v>
+      </c>
+      <c r="M6" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="N6" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="23"/>
-      <c r="R6" s="23"/>
-      <c r="S6" s="23"/>
-      <c r="T6" s="23"/>
-      <c r="U6" s="23"/>
-      <c r="BC6" s="9" t="str">
+      <c r="N6" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="20"/>
+      <c r="S6" s="20"/>
+      <c r="T6" s="20"/>
+      <c r="U6" s="20"/>
+      <c r="W6" s="20"/>
+      <c r="X6" s="20"/>
+      <c r="Y6" s="20"/>
+      <c r="Z6" s="20"/>
+      <c r="AA6" s="20"/>
+      <c r="AB6" s="20"/>
+      <c r="AC6" s="20"/>
+      <c r="AD6" s="20"/>
+      <c r="AF6" s="20"/>
+      <c r="AG6" s="20"/>
+      <c r="AH6" s="20"/>
+      <c r="AI6" s="20"/>
+      <c r="AJ6" s="20"/>
+      <c r="AK6" s="20"/>
+      <c r="AL6" s="20"/>
+      <c r="AM6" s="20"/>
+      <c r="AO6" s="20"/>
+      <c r="AP6" s="20"/>
+      <c r="AQ6" s="20"/>
+      <c r="AR6" s="20"/>
+      <c r="AS6" s="20"/>
+      <c r="AT6" s="20"/>
+      <c r="AU6" s="20"/>
+      <c r="AV6" s="20"/>
+      <c r="AX6" s="20"/>
+      <c r="AY6" s="20"/>
+      <c r="AZ6" s="20"/>
+      <c r="BA6" s="20"/>
+      <c r="BB6" s="20"/>
+      <c r="BC6" s="20"/>
+      <c r="BD6" s="20"/>
+      <c r="BE6" s="20"/>
+      <c r="BG6" s="15" t="str">
         <f t="shared" si="0"/>
         <v>End Command</v>
       </c>
     </row>
-    <row r="7" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>73</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="11">
-        <v>0</v>
-      </c>
-      <c r="F7" s="12">
-        <v>0</v>
-      </c>
-      <c r="G7" s="12">
-        <v>0</v>
-      </c>
-      <c r="H7" s="12">
-        <v>0</v>
-      </c>
-      <c r="I7" s="12">
-        <v>0</v>
-      </c>
-      <c r="J7" s="12">
-        <v>0</v>
-      </c>
-      <c r="K7" s="12">
-        <v>1</v>
-      </c>
-      <c r="L7" s="12">
-        <v>1</v>
-      </c>
-      <c r="M7" s="16" t="s">
+      <c r="E7" s="27">
+        <v>0</v>
+      </c>
+      <c r="F7" s="16">
+        <v>0</v>
+      </c>
+      <c r="G7" s="16">
+        <v>0</v>
+      </c>
+      <c r="H7" s="16">
+        <v>0</v>
+      </c>
+      <c r="I7" s="16">
+        <v>0</v>
+      </c>
+      <c r="J7" s="16">
+        <v>0</v>
+      </c>
+      <c r="K7" s="16">
+        <v>1</v>
+      </c>
+      <c r="L7" s="16">
+        <v>1</v>
+      </c>
+      <c r="M7" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="N7" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="O7" s="23"/>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="23"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="23"/>
-      <c r="U7" s="23"/>
-      <c r="BC7" s="9" t="str">
+      <c r="N7" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="20"/>
+      <c r="U7" s="20"/>
+      <c r="W7" s="20"/>
+      <c r="X7" s="20"/>
+      <c r="Y7" s="20"/>
+      <c r="Z7" s="20"/>
+      <c r="AA7" s="20"/>
+      <c r="AB7" s="20"/>
+      <c r="AC7" s="20"/>
+      <c r="AD7" s="20"/>
+      <c r="AF7" s="20"/>
+      <c r="AG7" s="20"/>
+      <c r="AH7" s="20"/>
+      <c r="AI7" s="20"/>
+      <c r="AJ7" s="20"/>
+      <c r="AK7" s="20"/>
+      <c r="AL7" s="20"/>
+      <c r="AM7" s="20"/>
+      <c r="AO7" s="20"/>
+      <c r="AP7" s="20"/>
+      <c r="AQ7" s="20"/>
+      <c r="AR7" s="20"/>
+      <c r="AS7" s="20"/>
+      <c r="AT7" s="20"/>
+      <c r="AU7" s="20"/>
+      <c r="AV7" s="20"/>
+      <c r="AX7" s="20"/>
+      <c r="AY7" s="20"/>
+      <c r="AZ7" s="20"/>
+      <c r="BA7" s="20"/>
+      <c r="BB7" s="20"/>
+      <c r="BC7" s="20"/>
+      <c r="BD7" s="20"/>
+      <c r="BE7" s="20"/>
+      <c r="BG7" s="15" t="str">
         <f t="shared" si="0"/>
         <v>End Command</v>
       </c>
     </row>
-    <row r="8" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>73</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="17">
-        <v>0</v>
-      </c>
-      <c r="F8" s="18">
-        <v>0</v>
-      </c>
-      <c r="G8" s="18">
-        <v>0</v>
-      </c>
-      <c r="H8" s="18">
-        <v>0</v>
-      </c>
-      <c r="I8" s="18">
-        <v>0</v>
-      </c>
-      <c r="J8" s="18">
-        <v>1</v>
-      </c>
-      <c r="K8" s="18">
-        <v>0</v>
-      </c>
-      <c r="L8" s="18">
-        <v>0</v>
-      </c>
-      <c r="M8" s="19" t="s">
+      <c r="E8" s="24">
+        <v>0</v>
+      </c>
+      <c r="F8" s="25">
+        <v>0</v>
+      </c>
+      <c r="G8" s="25">
+        <v>0</v>
+      </c>
+      <c r="H8" s="25">
+        <v>0</v>
+      </c>
+      <c r="I8" s="25">
+        <v>0</v>
+      </c>
+      <c r="J8" s="25">
+        <v>1</v>
+      </c>
+      <c r="K8" s="25">
+        <v>0</v>
+      </c>
+      <c r="L8" s="25">
+        <v>0</v>
+      </c>
+      <c r="M8" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="N8" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="O8" s="23"/>
-      <c r="P8" s="23"/>
-      <c r="Q8" s="23"/>
-      <c r="R8" s="23"/>
-      <c r="S8" s="23"/>
-      <c r="T8" s="23"/>
-      <c r="U8" s="23"/>
-      <c r="BC8" s="9" t="str">
+      <c r="N8" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="20"/>
+      <c r="S8" s="20"/>
+      <c r="T8" s="20"/>
+      <c r="U8" s="20"/>
+      <c r="W8" s="20"/>
+      <c r="X8" s="20"/>
+      <c r="Y8" s="20"/>
+      <c r="Z8" s="20"/>
+      <c r="AA8" s="20"/>
+      <c r="AB8" s="20"/>
+      <c r="AC8" s="20"/>
+      <c r="AD8" s="20"/>
+      <c r="AF8" s="20"/>
+      <c r="AG8" s="20"/>
+      <c r="AH8" s="20"/>
+      <c r="AI8" s="20"/>
+      <c r="AJ8" s="20"/>
+      <c r="AK8" s="20"/>
+      <c r="AL8" s="20"/>
+      <c r="AM8" s="20"/>
+      <c r="AO8" s="20"/>
+      <c r="AP8" s="20"/>
+      <c r="AQ8" s="20"/>
+      <c r="AR8" s="20"/>
+      <c r="AS8" s="20"/>
+      <c r="AT8" s="20"/>
+      <c r="AU8" s="20"/>
+      <c r="AV8" s="20"/>
+      <c r="AX8" s="20"/>
+      <c r="AY8" s="20"/>
+      <c r="AZ8" s="20"/>
+      <c r="BA8" s="20"/>
+      <c r="BB8" s="20"/>
+      <c r="BC8" s="20"/>
+      <c r="BD8" s="20"/>
+      <c r="BE8" s="20"/>
+      <c r="BG8" s="15" t="str">
         <f t="shared" si="0"/>
         <v>End Command</v>
       </c>
     </row>
-    <row r="9" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="BC9" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="B10" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="22"/>
-      <c r="BC10" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+    <row r="9" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="9" t="s">
+      <c r="B9" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="13">
-        <v>0</v>
-      </c>
-      <c r="F11" s="14">
-        <v>0</v>
-      </c>
-      <c r="G11" s="14">
-        <v>0</v>
-      </c>
-      <c r="H11" s="14">
-        <v>1</v>
-      </c>
-      <c r="I11" s="14">
-        <v>0</v>
-      </c>
-      <c r="J11" s="14">
-        <v>0</v>
-      </c>
-      <c r="K11" s="14">
-        <v>0</v>
-      </c>
-      <c r="L11" s="14">
-        <v>1</v>
-      </c>
-      <c r="M11" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="BC11" s="9" t="str">
+      <c r="E9" s="27">
+        <v>0</v>
+      </c>
+      <c r="F9" s="16">
+        <v>0</v>
+      </c>
+      <c r="G9" s="16">
+        <v>0</v>
+      </c>
+      <c r="H9" s="16">
+        <v>0</v>
+      </c>
+      <c r="I9" s="16">
+        <v>0</v>
+      </c>
+      <c r="J9" s="16">
+        <v>1</v>
+      </c>
+      <c r="K9" s="16">
+        <v>0</v>
+      </c>
+      <c r="L9" s="16">
+        <v>1</v>
+      </c>
+      <c r="M9" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="N9" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="O9" s="21"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="21"/>
+      <c r="R9" s="21"/>
+      <c r="S9" s="21"/>
+      <c r="T9" s="21"/>
+      <c r="U9" s="21"/>
+      <c r="W9" s="20"/>
+      <c r="X9" s="20"/>
+      <c r="Y9" s="20"/>
+      <c r="Z9" s="20"/>
+      <c r="AA9" s="20"/>
+      <c r="AB9" s="20"/>
+      <c r="AC9" s="20"/>
+      <c r="AD9" s="20"/>
+      <c r="AF9" s="20"/>
+      <c r="AG9" s="20"/>
+      <c r="AH9" s="20"/>
+      <c r="AI9" s="20"/>
+      <c r="AJ9" s="20"/>
+      <c r="AK9" s="20"/>
+      <c r="AL9" s="20"/>
+      <c r="AM9" s="20"/>
+      <c r="AO9" s="20"/>
+      <c r="AP9" s="20"/>
+      <c r="AQ9" s="20"/>
+      <c r="AR9" s="20"/>
+      <c r="AS9" s="20"/>
+      <c r="AT9" s="20"/>
+      <c r="AU9" s="20"/>
+      <c r="AV9" s="20"/>
+      <c r="AX9" s="20"/>
+      <c r="AY9" s="20"/>
+      <c r="AZ9" s="20"/>
+      <c r="BA9" s="20"/>
+      <c r="BB9" s="20"/>
+      <c r="BC9" s="20"/>
+      <c r="BD9" s="20"/>
+      <c r="BE9" s="20"/>
+      <c r="BG9" s="15" t="str">
         <f t="shared" si="0"/>
         <v>End Command</v>
       </c>
     </row>
-    <row r="12" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+    <row r="10" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="9" t="s">
+      <c r="B10" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="11">
-        <v>0</v>
-      </c>
-      <c r="F12" s="12">
-        <v>0</v>
-      </c>
-      <c r="G12" s="12">
-        <v>0</v>
-      </c>
-      <c r="H12" s="12">
-        <v>1</v>
-      </c>
-      <c r="I12" s="12">
-        <v>0</v>
-      </c>
-      <c r="J12" s="12">
-        <v>0</v>
-      </c>
-      <c r="K12" s="12">
-        <v>1</v>
-      </c>
-      <c r="L12" s="12">
-        <v>0</v>
-      </c>
-      <c r="M12" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="BC12" s="9" t="str">
+      <c r="E10" s="24">
+        <v>0</v>
+      </c>
+      <c r="F10" s="25">
+        <v>0</v>
+      </c>
+      <c r="G10" s="25">
+        <v>0</v>
+      </c>
+      <c r="H10" s="25">
+        <v>0</v>
+      </c>
+      <c r="I10" s="25">
+        <v>0</v>
+      </c>
+      <c r="J10" s="25">
+        <v>1</v>
+      </c>
+      <c r="K10" s="25">
+        <v>0</v>
+      </c>
+      <c r="L10" s="22">
+        <v>1</v>
+      </c>
+      <c r="M10" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="N10" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="21"/>
+      <c r="R10" s="21"/>
+      <c r="S10" s="21"/>
+      <c r="T10" s="21"/>
+      <c r="U10" s="21"/>
+      <c r="W10" s="20"/>
+      <c r="X10" s="20"/>
+      <c r="Y10" s="20"/>
+      <c r="Z10" s="20"/>
+      <c r="AA10" s="20"/>
+      <c r="AB10" s="20"/>
+      <c r="AC10" s="20"/>
+      <c r="AD10" s="20"/>
+      <c r="AF10" s="20"/>
+      <c r="AG10" s="20"/>
+      <c r="AH10" s="20"/>
+      <c r="AI10" s="20"/>
+      <c r="AJ10" s="20"/>
+      <c r="AK10" s="20"/>
+      <c r="AL10" s="20"/>
+      <c r="AM10" s="20"/>
+      <c r="AO10" s="20"/>
+      <c r="AP10" s="20"/>
+      <c r="AQ10" s="20"/>
+      <c r="AR10" s="20"/>
+      <c r="AS10" s="20"/>
+      <c r="AT10" s="20"/>
+      <c r="AU10" s="20"/>
+      <c r="AV10" s="20"/>
+      <c r="AX10" s="20"/>
+      <c r="AY10" s="20"/>
+      <c r="AZ10" s="20"/>
+      <c r="BA10" s="20"/>
+      <c r="BB10" s="20"/>
+      <c r="BC10" s="20"/>
+      <c r="BD10" s="20"/>
+      <c r="BE10" s="20"/>
+      <c r="BG10" s="15" t="str">
         <f t="shared" si="0"/>
         <v>End Command</v>
       </c>
     </row>
-    <row r="13" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="BG11" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="B12" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="19"/>
+      <c r="BG12" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>73</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="17">
-        <v>0</v>
-      </c>
-      <c r="F13" s="18">
-        <v>0</v>
-      </c>
-      <c r="G13" s="18">
-        <v>0</v>
-      </c>
-      <c r="H13" s="18">
-        <v>1</v>
-      </c>
-      <c r="I13" s="18">
-        <v>0</v>
-      </c>
-      <c r="J13" s="18">
-        <v>0</v>
-      </c>
-      <c r="K13" s="18">
-        <v>1</v>
-      </c>
-      <c r="L13" s="18">
-        <v>1</v>
-      </c>
-      <c r="M13" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="BC13" s="9" t="str">
+      <c r="E13" s="26">
+        <v>0</v>
+      </c>
+      <c r="F13" s="23">
+        <v>0</v>
+      </c>
+      <c r="G13" s="23">
+        <v>0</v>
+      </c>
+      <c r="H13" s="23">
+        <v>1</v>
+      </c>
+      <c r="I13" s="23">
+        <v>0</v>
+      </c>
+      <c r="J13" s="23">
+        <v>0</v>
+      </c>
+      <c r="K13" s="23">
+        <v>0</v>
+      </c>
+      <c r="L13" s="23">
+        <v>1</v>
+      </c>
+      <c r="M13" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BG13" s="15" t="str">
         <f t="shared" si="0"/>
         <v>End Command</v>
       </c>
     </row>
-    <row r="14" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="BC14" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D15" s="9" t="s">
+    <row r="14" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="21"/>
-      <c r="N15" s="21"/>
-      <c r="O15" s="21"/>
-      <c r="P15" s="21"/>
-      <c r="Q15" s="21"/>
-      <c r="R15" s="21"/>
-      <c r="S15" s="21"/>
-      <c r="T15" s="21"/>
-      <c r="U15" s="21"/>
-      <c r="V15" s="22"/>
-      <c r="BC15" s="9" t="str">
+      <c r="E14" s="27">
+        <v>0</v>
+      </c>
+      <c r="F14" s="16">
+        <v>0</v>
+      </c>
+      <c r="G14" s="16">
+        <v>0</v>
+      </c>
+      <c r="H14" s="16">
+        <v>1</v>
+      </c>
+      <c r="I14" s="16">
+        <v>0</v>
+      </c>
+      <c r="J14" s="16">
+        <v>0</v>
+      </c>
+      <c r="K14" s="16">
+        <v>1</v>
+      </c>
+      <c r="L14" s="16">
+        <v>0</v>
+      </c>
+      <c r="M14" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="BG14" s="15" t="str">
         <f t="shared" si="0"/>
         <v>End Command</v>
       </c>
     </row>
-    <row r="16" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="BC16" s="9" t="str">
+    <row r="15" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="24">
+        <v>0</v>
+      </c>
+      <c r="F15" s="25">
+        <v>0</v>
+      </c>
+      <c r="G15" s="25">
+        <v>0</v>
+      </c>
+      <c r="H15" s="25">
+        <v>1</v>
+      </c>
+      <c r="I15" s="25">
+        <v>0</v>
+      </c>
+      <c r="J15" s="25">
+        <v>0</v>
+      </c>
+      <c r="K15" s="25">
+        <v>1</v>
+      </c>
+      <c r="L15" s="25">
+        <v>1</v>
+      </c>
+      <c r="M15" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="BG15" s="15" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="7:55" x14ac:dyDescent="0.25">
-      <c r="BC17" s="9" t="str">
+        <v>End Command</v>
+      </c>
+    </row>
+    <row r="16" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="18"/>
+      <c r="Q16" s="18"/>
+      <c r="R16" s="18"/>
+      <c r="S16" s="18"/>
+      <c r="T16" s="18"/>
+      <c r="U16" s="18"/>
+      <c r="V16" s="19"/>
+      <c r="BG16" s="15" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="7:55" x14ac:dyDescent="0.25">
-      <c r="BC18" s="9" t="str">
+        <v>End Command</v>
+      </c>
+    </row>
+    <row r="17" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+      <c r="S17" s="16"/>
+      <c r="T17" s="16"/>
+      <c r="U17" s="16"/>
+      <c r="V17" s="16"/>
+    </row>
+    <row r="18" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="B18" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="29"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="O19" s="20"/>
+      <c r="P19" s="20"/>
+      <c r="Q19" s="20"/>
+      <c r="R19" s="20"/>
+      <c r="S19" s="20"/>
+      <c r="T19" s="20"/>
+      <c r="U19" s="20"/>
+      <c r="V19" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="BG19" s="15" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="7:55" x14ac:dyDescent="0.25">
-      <c r="BC19" s="9" t="str">
+        <v>End Command</v>
+      </c>
+    </row>
+    <row r="20" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="31"/>
+      <c r="L20" s="31"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="21"/>
+      <c r="O20" s="21"/>
+      <c r="P20" s="21"/>
+      <c r="Q20" s="21"/>
+      <c r="R20" s="21"/>
+      <c r="S20" s="21"/>
+      <c r="T20" s="21"/>
+      <c r="U20" s="21"/>
+      <c r="V20" s="16"/>
+      <c r="BG20" s="15" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="7:55" x14ac:dyDescent="0.25">
-      <c r="BC20" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="7:55" x14ac:dyDescent="0.25">
-      <c r="G21" s="12">
-        <v>0</v>
-      </c>
-      <c r="H21" s="12">
-        <v>0</v>
-      </c>
-      <c r="I21" s="12">
-        <v>0</v>
-      </c>
-      <c r="J21" s="12">
-        <v>0</v>
-      </c>
-      <c r="M21" s="10" t="s">
+        <v>End Command</v>
+      </c>
+    </row>
+    <row r="21" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="BG21" s="15" t="str">
+        <f>IF($D21 = "Start Command", "End Command", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="B22" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="A23" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="18"/>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="18"/>
+      <c r="S23" s="18"/>
+      <c r="T23" s="18"/>
+      <c r="U23" s="18"/>
+      <c r="V23" s="19"/>
+    </row>
+    <row r="24" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="B24" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="E24" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="29"/>
+    </row>
+    <row r="26" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="BG26" s="15" t="str">
+        <f>IF($D26 = "Start Command", "End Command", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="BG27" s="15" t="str">
+        <f>IF($D27 = "Start Command", "End Command", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="G28" s="16">
+        <v>0</v>
+      </c>
+      <c r="H28" s="16">
+        <v>0</v>
+      </c>
+      <c r="I28" s="16">
+        <v>0</v>
+      </c>
+      <c r="J28" s="16">
+        <v>0</v>
+      </c>
+      <c r="M28" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="BC21" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="7:55" x14ac:dyDescent="0.25">
-      <c r="G22" s="12">
-        <v>0</v>
-      </c>
-      <c r="H22" s="12">
-        <v>0</v>
-      </c>
-      <c r="I22" s="12">
-        <v>0</v>
-      </c>
-      <c r="J22" s="12">
-        <v>1</v>
-      </c>
-      <c r="M22" s="10" t="s">
+      <c r="BG28" s="15" t="str">
+        <f>IF($D28 = "Start Command", "End Command", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="G29" s="16">
+        <v>0</v>
+      </c>
+      <c r="H29" s="16">
+        <v>0</v>
+      </c>
+      <c r="I29" s="16">
+        <v>0</v>
+      </c>
+      <c r="J29" s="16">
+        <v>1</v>
+      </c>
+      <c r="M29" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="BC22" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="7:55" x14ac:dyDescent="0.25">
-      <c r="G23" s="12">
-        <v>0</v>
-      </c>
-      <c r="H23" s="12">
-        <v>0</v>
-      </c>
-      <c r="I23" s="12">
-        <v>1</v>
-      </c>
-      <c r="J23" s="12">
-        <v>0</v>
-      </c>
-      <c r="M23" s="10" t="s">
+      <c r="BG29" s="15" t="str">
+        <f>IF($D29 = "Start Command", "End Command", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="G30" s="16">
+        <v>0</v>
+      </c>
+      <c r="H30" s="16">
+        <v>0</v>
+      </c>
+      <c r="I30" s="16">
+        <v>1</v>
+      </c>
+      <c r="J30" s="16">
+        <v>0</v>
+      </c>
+      <c r="M30" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="BC23" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="7:55" x14ac:dyDescent="0.25">
-      <c r="G24" s="12">
-        <v>0</v>
-      </c>
-      <c r="H24" s="12">
-        <v>0</v>
-      </c>
-      <c r="I24" s="12">
-        <v>1</v>
-      </c>
-      <c r="J24" s="12">
-        <v>1</v>
-      </c>
-      <c r="M24" s="10" t="s">
+      <c r="BG30" s="15" t="str">
+        <f>IF($D30 = "Start Command", "End Command", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="G31" s="16">
+        <v>0</v>
+      </c>
+      <c r="H31" s="16">
+        <v>0</v>
+      </c>
+      <c r="I31" s="16">
+        <v>1</v>
+      </c>
+      <c r="J31" s="16">
+        <v>1</v>
+      </c>
+      <c r="M31" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="BC24" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="7:55" x14ac:dyDescent="0.25">
-      <c r="G25" s="12">
-        <v>0</v>
-      </c>
-      <c r="H25" s="12">
-        <v>1</v>
-      </c>
-      <c r="I25" s="12">
-        <v>0</v>
-      </c>
-      <c r="J25" s="12">
-        <v>0</v>
-      </c>
-      <c r="M25" s="10" t="s">
+      <c r="BG31" s="15" t="str">
+        <f>IF($D31 = "Start Command", "End Command", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="G32" s="16">
+        <v>0</v>
+      </c>
+      <c r="H32" s="16">
+        <v>1</v>
+      </c>
+      <c r="I32" s="16">
+        <v>0</v>
+      </c>
+      <c r="J32" s="16">
+        <v>0</v>
+      </c>
+      <c r="M32" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="BC25" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="7:55" x14ac:dyDescent="0.25">
-      <c r="G26" s="12">
-        <v>0</v>
-      </c>
-      <c r="H26" s="12">
-        <v>1</v>
-      </c>
-      <c r="I26" s="12">
-        <v>0</v>
-      </c>
-      <c r="J26" s="12">
-        <v>1</v>
-      </c>
-      <c r="M26" s="10" t="s">
+      <c r="BG32" s="15" t="str">
+        <f>IF($D32 = "Start Command", "End Command", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="7:59" x14ac:dyDescent="0.3">
+      <c r="G33" s="16">
+        <v>0</v>
+      </c>
+      <c r="H33" s="16">
+        <v>1</v>
+      </c>
+      <c r="I33" s="16">
+        <v>0</v>
+      </c>
+      <c r="J33" s="16">
+        <v>1</v>
+      </c>
+      <c r="M33" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="BC26" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="7:55" x14ac:dyDescent="0.25">
-      <c r="G27" s="12">
-        <v>0</v>
-      </c>
-      <c r="H27" s="12">
-        <v>1</v>
-      </c>
-      <c r="I27" s="12">
-        <v>1</v>
-      </c>
-      <c r="J27" s="12">
-        <v>0</v>
-      </c>
-      <c r="M27" s="10" t="s">
+      <c r="BG33" s="15" t="str">
+        <f>IF($D33 = "Start Command", "End Command", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="7:59" x14ac:dyDescent="0.3">
+      <c r="G34" s="16">
+        <v>0</v>
+      </c>
+      <c r="H34" s="16">
+        <v>1</v>
+      </c>
+      <c r="I34" s="16">
+        <v>1</v>
+      </c>
+      <c r="J34" s="16">
+        <v>0</v>
+      </c>
+      <c r="M34" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="BC27" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="7:55" x14ac:dyDescent="0.25">
-      <c r="G28" s="12">
-        <v>0</v>
-      </c>
-      <c r="H28" s="12">
-        <v>1</v>
-      </c>
-      <c r="I28" s="12">
-        <v>1</v>
-      </c>
-      <c r="J28" s="12">
-        <v>1</v>
-      </c>
-      <c r="M28" s="10" t="s">
+      <c r="BG34" s="15" t="str">
+        <f>IF($D34 = "Start Command", "End Command", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="7:59" x14ac:dyDescent="0.3">
+      <c r="G35" s="16">
+        <v>0</v>
+      </c>
+      <c r="H35" s="16">
+        <v>1</v>
+      </c>
+      <c r="I35" s="16">
+        <v>1</v>
+      </c>
+      <c r="J35" s="16">
+        <v>1</v>
+      </c>
+      <c r="M35" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="BC28" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="7:55" x14ac:dyDescent="0.25">
-      <c r="G29" s="12">
-        <v>1</v>
-      </c>
-      <c r="H29" s="12">
-        <v>0</v>
-      </c>
-      <c r="I29" s="12">
-        <v>0</v>
-      </c>
-      <c r="J29" s="12">
-        <v>0</v>
-      </c>
-      <c r="M29" s="10" t="s">
+      <c r="BG35" s="15" t="str">
+        <f>IF($D35 = "Start Command", "End Command", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="7:59" x14ac:dyDescent="0.3">
+      <c r="G36" s="16">
+        <v>1</v>
+      </c>
+      <c r="H36" s="16">
+        <v>0</v>
+      </c>
+      <c r="I36" s="16">
+        <v>0</v>
+      </c>
+      <c r="J36" s="16">
+        <v>0</v>
+      </c>
+      <c r="M36" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="BC29" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="30" spans="7:55" x14ac:dyDescent="0.25">
-      <c r="G30" s="12">
-        <v>1</v>
-      </c>
-      <c r="H30" s="12">
-        <v>0</v>
-      </c>
-      <c r="I30" s="12">
-        <v>0</v>
-      </c>
-      <c r="J30" s="12">
-        <v>1</v>
-      </c>
-      <c r="M30" s="10" t="s">
+      <c r="BG36" s="15" t="str">
+        <f>IF($D36 = "Start Command", "End Command", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="7:59" x14ac:dyDescent="0.3">
+      <c r="G37" s="16">
+        <v>1</v>
+      </c>
+      <c r="H37" s="16">
+        <v>0</v>
+      </c>
+      <c r="I37" s="16">
+        <v>0</v>
+      </c>
+      <c r="J37" s="16">
+        <v>1</v>
+      </c>
+      <c r="M37" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="BC30" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="7:55" x14ac:dyDescent="0.25">
-      <c r="G31" s="12">
-        <v>1</v>
-      </c>
-      <c r="H31" s="12">
-        <v>0</v>
-      </c>
-      <c r="I31" s="12">
-        <v>1</v>
-      </c>
-      <c r="J31" s="12">
-        <v>0</v>
-      </c>
-      <c r="M31" s="10" t="s">
+      <c r="BG37" s="15" t="str">
+        <f>IF($D37 = "Start Command", "End Command", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="7:59" x14ac:dyDescent="0.3">
+      <c r="G38" s="16">
+        <v>1</v>
+      </c>
+      <c r="H38" s="16">
+        <v>0</v>
+      </c>
+      <c r="I38" s="16">
+        <v>1</v>
+      </c>
+      <c r="J38" s="16">
+        <v>0</v>
+      </c>
+      <c r="M38" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="BC31" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="7:55" x14ac:dyDescent="0.25">
-      <c r="G32" s="12">
-        <v>1</v>
-      </c>
-      <c r="H32" s="12">
-        <v>0</v>
-      </c>
-      <c r="I32" s="12">
-        <v>1</v>
-      </c>
-      <c r="J32" s="12">
-        <v>1</v>
-      </c>
-      <c r="M32" s="10" t="s">
+      <c r="BG38" s="15" t="str">
+        <f>IF($D38 = "Start Command", "End Command", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="7:59" x14ac:dyDescent="0.3">
+      <c r="G39" s="16">
+        <v>1</v>
+      </c>
+      <c r="H39" s="16">
+        <v>0</v>
+      </c>
+      <c r="I39" s="16">
+        <v>1</v>
+      </c>
+      <c r="J39" s="16">
+        <v>1</v>
+      </c>
+      <c r="M39" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="BC32" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="7:55" x14ac:dyDescent="0.25">
-      <c r="G33" s="12">
-        <v>1</v>
-      </c>
-      <c r="H33" s="12">
-        <v>1</v>
-      </c>
-      <c r="I33" s="12">
-        <v>0</v>
-      </c>
-      <c r="J33" s="12">
-        <v>0</v>
-      </c>
-      <c r="M33" s="10" t="s">
+      <c r="BG39" s="15" t="str">
+        <f>IF($D39 = "Start Command", "End Command", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="7:59" x14ac:dyDescent="0.3">
+      <c r="G40" s="16">
+        <v>1</v>
+      </c>
+      <c r="H40" s="16">
+        <v>1</v>
+      </c>
+      <c r="I40" s="16">
+        <v>0</v>
+      </c>
+      <c r="J40" s="16">
+        <v>0</v>
+      </c>
+      <c r="M40" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="BC33" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="7:55" x14ac:dyDescent="0.25">
-      <c r="G34" s="12">
-        <v>1</v>
-      </c>
-      <c r="H34" s="12">
-        <v>1</v>
-      </c>
-      <c r="I34" s="12">
-        <v>0</v>
-      </c>
-      <c r="J34" s="12">
-        <v>1</v>
-      </c>
-      <c r="M34" s="10" t="s">
+      <c r="BG40" s="15" t="str">
+        <f>IF($D40 = "Start Command", "End Command", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="7:59" x14ac:dyDescent="0.3">
+      <c r="G41" s="16">
+        <v>1</v>
+      </c>
+      <c r="H41" s="16">
+        <v>1</v>
+      </c>
+      <c r="I41" s="16">
+        <v>0</v>
+      </c>
+      <c r="J41" s="16">
+        <v>1</v>
+      </c>
+      <c r="M41" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="BC34" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="7:55" x14ac:dyDescent="0.25">
-      <c r="G35" s="12">
-        <v>1</v>
-      </c>
-      <c r="H35" s="12">
-        <v>1</v>
-      </c>
-      <c r="I35" s="12">
-        <v>1</v>
-      </c>
-      <c r="J35" s="12">
-        <v>0</v>
-      </c>
-      <c r="M35" s="10" t="s">
+      <c r="BG41" s="15" t="str">
+        <f>IF($D41 = "Start Command", "End Command", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="7:59" x14ac:dyDescent="0.3">
+      <c r="G42" s="16">
+        <v>1</v>
+      </c>
+      <c r="H42" s="16">
+        <v>1</v>
+      </c>
+      <c r="I42" s="16">
+        <v>1</v>
+      </c>
+      <c r="J42" s="16">
+        <v>0</v>
+      </c>
+      <c r="M42" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="BC35" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="36" spans="7:55" x14ac:dyDescent="0.25">
-      <c r="G36" s="12">
-        <v>1</v>
-      </c>
-      <c r="H36" s="12">
-        <v>1</v>
-      </c>
-      <c r="I36" s="12">
-        <v>1</v>
-      </c>
-      <c r="J36" s="12">
-        <v>1</v>
-      </c>
-      <c r="M36" s="10" t="s">
+      <c r="BG42" s="15" t="str">
+        <f>IF($D42 = "Start Command", "End Command", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="7:59" x14ac:dyDescent="0.3">
+      <c r="G43" s="16">
+        <v>1</v>
+      </c>
+      <c r="H43" s="16">
+        <v>1</v>
+      </c>
+      <c r="I43" s="16">
+        <v>1</v>
+      </c>
+      <c r="J43" s="16">
+        <v>1</v>
+      </c>
+      <c r="M43" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="BC36" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="7:55" x14ac:dyDescent="0.25">
-      <c r="BC37" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="38" spans="7:55" x14ac:dyDescent="0.25">
-      <c r="BC38" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="39" spans="7:55" x14ac:dyDescent="0.25">
-      <c r="BC39" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="40" spans="7:55" x14ac:dyDescent="0.25">
-      <c r="BC40" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="41" spans="7:55" x14ac:dyDescent="0.25">
-      <c r="BC41" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="42" spans="7:55" x14ac:dyDescent="0.25">
-      <c r="BC42" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="43" spans="7:55" x14ac:dyDescent="0.25">
-      <c r="BC43" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="44" spans="7:55" x14ac:dyDescent="0.25">
-      <c r="BC44" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="45" spans="7:55" x14ac:dyDescent="0.25">
-      <c r="BC45" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="46" spans="7:55" x14ac:dyDescent="0.25">
-      <c r="BC46" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="47" spans="7:55" x14ac:dyDescent="0.25">
-      <c r="BC47" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="48" spans="7:55" x14ac:dyDescent="0.25">
-      <c r="BC48" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="49" spans="55:55" x14ac:dyDescent="0.25">
-      <c r="BC49" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="50" spans="55:55" x14ac:dyDescent="0.25">
-      <c r="BC50" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="51" spans="55:55" x14ac:dyDescent="0.25">
-      <c r="BC51" s="9" t="str">
-        <f t="shared" si="0"/>
+      <c r="BG43" s="15" t="str">
+        <f>IF($D43 = "Start Command", "End Command", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="7:59" x14ac:dyDescent="0.3">
+      <c r="BG44" s="15" t="str">
+        <f>IF($D44 = "Start Command", "End Command", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="7:59" x14ac:dyDescent="0.3">
+      <c r="BG45" s="15" t="str">
+        <f>IF($D45 = "Start Command", "End Command", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="7:59" x14ac:dyDescent="0.3">
+      <c r="BG46" s="15" t="str">
+        <f>IF($D46 = "Start Command", "End Command", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="7:59" x14ac:dyDescent="0.3">
+      <c r="BG47" s="15" t="str">
+        <f>IF($D47 = "Start Command", "End Command", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="7:59" x14ac:dyDescent="0.3">
+      <c r="BG48" s="15" t="str">
+        <f>IF($D48 = "Start Command", "End Command", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="59:59" x14ac:dyDescent="0.3">
+      <c r="BG49" s="15" t="str">
+        <f>IF($D49 = "Start Command", "End Command", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="59:59" x14ac:dyDescent="0.3">
+      <c r="BG50" s="15" t="str">
+        <f>IF($D50 = "Start Command", "End Command", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="59:59" x14ac:dyDescent="0.3">
+      <c r="BG51" s="15" t="str">
+        <f>IF($D51 = "Start Command", "End Command", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="59:59" x14ac:dyDescent="0.3">
+      <c r="BG52" s="15" t="str">
+        <f>IF($D52 = "Start Command", "End Command", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="59:59" x14ac:dyDescent="0.3">
+      <c r="BG53" s="15" t="str">
+        <f>IF($D53 = "Start Command", "End Command", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="59:59" x14ac:dyDescent="0.3">
+      <c r="BG54" s="15" t="str">
+        <f>IF($D54 = "Start Command", "End Command", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="59:59" x14ac:dyDescent="0.3">
+      <c r="BG55" s="15" t="str">
+        <f>IF($D55 = "Start Command", "End Command", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="59:59" x14ac:dyDescent="0.3">
+      <c r="BG56" s="15" t="str">
+        <f>IF($D56 = "Start Command", "End Command", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="59:59" x14ac:dyDescent="0.3">
+      <c r="BG57" s="15" t="str">
+        <f>IF($D57 = "Start Command", "End Command", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="59:59" x14ac:dyDescent="0.3">
+      <c r="BG58" s="15" t="str">
+        <f>IF($D58 = "Start Command", "End Command", "")</f>
         <v/>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="E15:V15"/>
-    <mergeCell ref="AU1:BB1"/>
+  <mergeCells count="46">
+    <mergeCell ref="E24:L24"/>
+    <mergeCell ref="AX10:BE10"/>
+    <mergeCell ref="E23:V23"/>
+    <mergeCell ref="AO10:AV10"/>
+    <mergeCell ref="AF10:AM10"/>
+    <mergeCell ref="W10:AD10"/>
+    <mergeCell ref="N10:U10"/>
+    <mergeCell ref="N9:U9"/>
+    <mergeCell ref="AX5:BE5"/>
+    <mergeCell ref="AX6:BE6"/>
+    <mergeCell ref="AX7:BE7"/>
+    <mergeCell ref="AX8:BE8"/>
+    <mergeCell ref="AX9:BE9"/>
+    <mergeCell ref="AO5:AV5"/>
+    <mergeCell ref="AO6:AV6"/>
+    <mergeCell ref="AO7:AV7"/>
+    <mergeCell ref="AO8:AV8"/>
+    <mergeCell ref="AO9:AV9"/>
+    <mergeCell ref="W6:AD6"/>
+    <mergeCell ref="W7:AD7"/>
+    <mergeCell ref="W8:AD8"/>
+    <mergeCell ref="W9:AD9"/>
+    <mergeCell ref="AF5:AM5"/>
+    <mergeCell ref="AF6:AM6"/>
+    <mergeCell ref="AF7:AM7"/>
+    <mergeCell ref="AF8:AM8"/>
+    <mergeCell ref="AF9:AM9"/>
+    <mergeCell ref="N8:U8"/>
+    <mergeCell ref="E19:L19"/>
+    <mergeCell ref="E20:L20"/>
+    <mergeCell ref="N19:U19"/>
+    <mergeCell ref="N20:U20"/>
+    <mergeCell ref="E16:V16"/>
+    <mergeCell ref="AX1:BE1"/>
     <mergeCell ref="E4:H4"/>
-    <mergeCell ref="E10:H10"/>
-    <mergeCell ref="N5:U5"/>
+    <mergeCell ref="E12:H12"/>
     <mergeCell ref="N6:U6"/>
     <mergeCell ref="N7:U7"/>
-    <mergeCell ref="N8:U8"/>
+    <mergeCell ref="N5:U5"/>
     <mergeCell ref="I4:L4"/>
-    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="I12:L12"/>
     <mergeCell ref="E1:L1"/>
     <mergeCell ref="N1:U1"/>
     <mergeCell ref="W1:AD1"/>
-    <mergeCell ref="AE1:AL1"/>
-    <mergeCell ref="AM1:AT1"/>
+    <mergeCell ref="AF1:AM1"/>
+    <mergeCell ref="AO1:AV1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1862,17 +2457,17 @@
       <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="9.140625" style="1"/>
-    <col min="10" max="10" width="10.5703125" style="1" customWidth="1"/>
-    <col min="11" max="13" width="10.5703125" style="7" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="2"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="22.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="9.109375" style="1"/>
+    <col min="10" max="10" width="10.5546875" style="1" customWidth="1"/>
+    <col min="11" max="13" width="10.5546875" style="7" customWidth="1"/>
+    <col min="14" max="14" width="9.109375" style="2"/>
+    <col min="15" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1910,7 +2505,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -1944,7 +2539,7 @@
       <c r="AC2" s="8"/>
       <c r="AD2" s="8"/>
     </row>
-    <row r="3" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1962,7 +2557,7 @@
       </c>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -1992,7 +2587,7 @@
       </c>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -2025,7 +2620,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -2058,7 +2653,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
@@ -2091,7 +2686,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -2124,7 +2719,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
@@ -2157,7 +2752,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -2190,7 +2785,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
@@ -2223,7 +2818,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
@@ -2256,7 +2851,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -2276,7 +2871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -2296,7 +2891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -2316,7 +2911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -2336,7 +2931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -2356,7 +2951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -2376,7 +2971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -2396,7 +2991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -2408,7 +3003,7 @@
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -2420,7 +3015,7 @@
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -2432,7 +3027,7 @@
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
     </row>
-    <row r="24" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>3</v>
       </c>
@@ -2450,7 +3045,7 @@
       </c>
       <c r="N24" s="2"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>15</v>
       </c>
@@ -2482,7 +3077,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>16</v>
       </c>
@@ -2514,7 +3109,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>17</v>
       </c>
@@ -2546,7 +3141,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>18</v>
       </c>
@@ -2578,7 +3173,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>19</v>
       </c>
@@ -2610,7 +3205,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="G30" s="4">
         <v>0</v>
@@ -2625,7 +3220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="G31" s="4">
         <v>0</v>
@@ -2640,7 +3235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="G32" s="4">
         <v>0</v>
@@ -2655,7 +3250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="G33" s="4">
         <v>1</v>
@@ -2670,7 +3265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="G34" s="4">
         <v>1</v>
@@ -2685,7 +3280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="G35" s="4">
         <v>1</v>
@@ -2700,7 +3295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="G36" s="4">
         <v>1</v>
@@ -2715,7 +3310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="G37" s="4">
         <v>1</v>
@@ -2730,7 +3325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="G38" s="4">
         <v>1</v>
@@ -2745,7 +3340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="G39" s="4">
         <v>1</v>
@@ -2760,7 +3355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="4"/>
       <c r="G40" s="4">
         <v>1</v>

</xml_diff>